<commit_message>
added column for status as of July 4, 2025
</commit_message>
<xml_diff>
--- a/Filtered_By_Region/BARMM/BARMM_NEWCON.xlsx
+++ b/Filtered_By_Region/BARMM/BARMM_NEWCON.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="DropdownOptions" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS48"/>
+  <dimension ref="A1:AT48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,6 +660,11 @@
           <t>Project Allocation (original)</t>
         </is>
       </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>Status as of July 4, 2025</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -697,7 +703,6 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
           <t>1-UNIT 4STY</t>
@@ -711,8 +716,6 @@
       <c r="L2" t="n">
         <v>40000000</v>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -721,17 +724,6 @@
       <c r="P2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="n">
         <v>0</v>
       </c>
@@ -747,7 +739,6 @@
       <c r="AF2" t="n">
         <v>0</v>
       </c>
-      <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="n">
         <v>0</v>
       </c>
@@ -763,17 +754,12 @@
       <c r="AL2" t="n">
         <v>0</v>
       </c>
-      <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="n">
         <v>0</v>
       </c>
       <c r="AO2" t="n">
         <v>0</v>
       </c>
-      <c r="AP2" t="inlineStr"/>
-      <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="inlineStr"/>
-      <c r="AS2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -828,8 +814,6 @@
       <c r="L3" t="n">
         <v>40000000</v>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -838,17 +822,6 @@
       <c r="P3" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="n">
         <v>0</v>
       </c>
@@ -864,7 +837,6 @@
       <c r="AF3" t="n">
         <v>0</v>
       </c>
-      <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="n">
         <v>0</v>
       </c>
@@ -880,17 +852,12 @@
       <c r="AL3" t="n">
         <v>0</v>
       </c>
-      <c r="AM3" t="inlineStr"/>
       <c r="AN3" t="n">
         <v>0</v>
       </c>
       <c r="AO3" t="n">
         <v>0</v>
       </c>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="inlineStr"/>
-      <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -911,7 +878,6 @@
       <c r="D4" t="n">
         <v>133540</v>
       </c>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
           <t>BUMBARAN</t>
@@ -941,8 +907,6 @@
       <c r="L4" t="n">
         <v>10000000</v>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -951,17 +915,6 @@
       <c r="P4" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="n">
         <v>0</v>
       </c>
@@ -977,7 +930,6 @@
       <c r="AF4" t="n">
         <v>0</v>
       </c>
-      <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="n">
         <v>0</v>
       </c>
@@ -993,17 +945,12 @@
       <c r="AL4" t="n">
         <v>0</v>
       </c>
-      <c r="AM4" t="inlineStr"/>
       <c r="AN4" t="n">
         <v>0</v>
       </c>
       <c r="AO4" t="n">
         <v>0</v>
       </c>
-      <c r="AP4" t="inlineStr"/>
-      <c r="AQ4" t="inlineStr"/>
-      <c r="AR4" t="inlineStr"/>
-      <c r="AS4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1058,8 +1005,6 @@
       <c r="L5" t="n">
         <v>10000000</v>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -1068,17 +1013,6 @@
       <c r="P5" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="n">
         <v>0</v>
       </c>
@@ -1094,7 +1028,6 @@
       <c r="AF5" t="n">
         <v>0</v>
       </c>
-      <c r="AG5" t="inlineStr"/>
       <c r="AH5" t="n">
         <v>0</v>
       </c>
@@ -1110,17 +1043,12 @@
       <c r="AL5" t="n">
         <v>0</v>
       </c>
-      <c r="AM5" t="inlineStr"/>
       <c r="AN5" t="n">
         <v>0</v>
       </c>
       <c r="AO5" t="n">
         <v>0</v>
       </c>
-      <c r="AP5" t="inlineStr"/>
-      <c r="AQ5" t="inlineStr"/>
-      <c r="AR5" t="inlineStr"/>
-      <c r="AS5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1175,8 +1103,6 @@
       <c r="L6" t="n">
         <v>30000000</v>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -1185,17 +1111,6 @@
       <c r="P6" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="n">
         <v>0</v>
       </c>
@@ -1211,7 +1126,6 @@
       <c r="AF6" t="n">
         <v>0</v>
       </c>
-      <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="n">
         <v>0</v>
       </c>
@@ -1227,17 +1141,12 @@
       <c r="AL6" t="n">
         <v>0</v>
       </c>
-      <c r="AM6" t="inlineStr"/>
       <c r="AN6" t="n">
         <v>0</v>
       </c>
       <c r="AO6" t="n">
         <v>0</v>
       </c>
-      <c r="AP6" t="inlineStr"/>
-      <c r="AQ6" t="inlineStr"/>
-      <c r="AR6" t="inlineStr"/>
-      <c r="AS6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1292,8 +1201,6 @@
       <c r="L7" t="n">
         <v>30000000</v>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -1302,17 +1209,6 @@
       <c r="P7" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="n">
         <v>0</v>
       </c>
@@ -1328,7 +1224,6 @@
       <c r="AF7" t="n">
         <v>0</v>
       </c>
-      <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="n">
         <v>0</v>
       </c>
@@ -1344,17 +1239,12 @@
       <c r="AL7" t="n">
         <v>0</v>
       </c>
-      <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="n">
         <v>0</v>
       </c>
       <c r="AO7" t="n">
         <v>0</v>
       </c>
-      <c r="AP7" t="inlineStr"/>
-      <c r="AQ7" t="inlineStr"/>
-      <c r="AR7" t="inlineStr"/>
-      <c r="AS7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1409,8 +1299,6 @@
       <c r="L8" t="n">
         <v>10000000</v>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -1419,17 +1307,6 @@
       <c r="P8" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="n">
         <v>0</v>
       </c>
@@ -1445,7 +1322,6 @@
       <c r="AF8" t="n">
         <v>0</v>
       </c>
-      <c r="AG8" t="inlineStr"/>
       <c r="AH8" t="n">
         <v>0</v>
       </c>
@@ -1461,17 +1337,12 @@
       <c r="AL8" t="n">
         <v>0</v>
       </c>
-      <c r="AM8" t="inlineStr"/>
       <c r="AN8" t="n">
         <v>0</v>
       </c>
       <c r="AO8" t="n">
         <v>0</v>
       </c>
-      <c r="AP8" t="inlineStr"/>
-      <c r="AQ8" t="inlineStr"/>
-      <c r="AR8" t="inlineStr"/>
-      <c r="AS8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1526,8 +1397,6 @@
       <c r="L9" t="n">
         <v>42000000</v>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -1536,17 +1405,6 @@
       <c r="P9" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="n">
         <v>0</v>
       </c>
@@ -1562,7 +1420,6 @@
       <c r="AF9" t="n">
         <v>0</v>
       </c>
-      <c r="AG9" t="inlineStr"/>
       <c r="AH9" t="n">
         <v>0</v>
       </c>
@@ -1578,17 +1435,12 @@
       <c r="AL9" t="n">
         <v>0</v>
       </c>
-      <c r="AM9" t="inlineStr"/>
       <c r="AN9" t="n">
         <v>0</v>
       </c>
       <c r="AO9" t="n">
         <v>0</v>
       </c>
-      <c r="AP9" t="inlineStr"/>
-      <c r="AQ9" t="inlineStr"/>
-      <c r="AR9" t="inlineStr"/>
-      <c r="AS9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1643,8 +1495,6 @@
       <c r="L10" t="n">
         <v>10000000</v>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -1653,17 +1503,6 @@
       <c r="P10" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="n">
         <v>0</v>
       </c>
@@ -1679,7 +1518,6 @@
       <c r="AF10" t="n">
         <v>0</v>
       </c>
-      <c r="AG10" t="inlineStr"/>
       <c r="AH10" t="n">
         <v>0</v>
       </c>
@@ -1695,17 +1533,12 @@
       <c r="AL10" t="n">
         <v>0</v>
       </c>
-      <c r="AM10" t="inlineStr"/>
       <c r="AN10" t="n">
         <v>0</v>
       </c>
       <c r="AO10" t="n">
         <v>0</v>
       </c>
-      <c r="AP10" t="inlineStr"/>
-      <c r="AQ10" t="inlineStr"/>
-      <c r="AR10" t="inlineStr"/>
-      <c r="AS10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1760,8 +1593,6 @@
       <c r="L11" t="n">
         <v>10000000</v>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -1770,17 +1601,6 @@
       <c r="P11" t="n">
         <v>0</v>
       </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="n">
         <v>0</v>
       </c>
@@ -1796,7 +1616,6 @@
       <c r="AF11" t="n">
         <v>0</v>
       </c>
-      <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="n">
         <v>0</v>
       </c>
@@ -1812,17 +1631,12 @@
       <c r="AL11" t="n">
         <v>0</v>
       </c>
-      <c r="AM11" t="inlineStr"/>
       <c r="AN11" t="n">
         <v>0</v>
       </c>
       <c r="AO11" t="n">
         <v>0</v>
       </c>
-      <c r="AP11" t="inlineStr"/>
-      <c r="AQ11" t="inlineStr"/>
-      <c r="AR11" t="inlineStr"/>
-      <c r="AS11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1877,8 +1691,6 @@
       <c r="L12" t="n">
         <v>5000000</v>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -1887,17 +1699,6 @@
       <c r="P12" t="n">
         <v>0</v>
       </c>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="n">
         <v>0</v>
       </c>
@@ -1913,7 +1714,6 @@
       <c r="AF12" t="n">
         <v>0</v>
       </c>
-      <c r="AG12" t="inlineStr"/>
       <c r="AH12" t="n">
         <v>0</v>
       </c>
@@ -1929,17 +1729,12 @@
       <c r="AL12" t="n">
         <v>0</v>
       </c>
-      <c r="AM12" t="inlineStr"/>
       <c r="AN12" t="n">
         <v>0</v>
       </c>
       <c r="AO12" t="n">
         <v>0</v>
       </c>
-      <c r="AP12" t="inlineStr"/>
-      <c r="AQ12" t="inlineStr"/>
-      <c r="AR12" t="inlineStr"/>
-      <c r="AS12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1957,7 +1752,6 @@
           <t>Lanao del Sur - II</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
           <t>Pagayonan National High School</t>
@@ -1992,8 +1786,6 @@
       <c r="L13" t="n">
         <v>5000000</v>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -2002,17 +1794,6 @@
       <c r="P13" t="n">
         <v>0</v>
       </c>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="n">
         <v>0</v>
       </c>
@@ -2028,7 +1809,6 @@
       <c r="AF13" t="n">
         <v>0</v>
       </c>
-      <c r="AG13" t="inlineStr"/>
       <c r="AH13" t="n">
         <v>0</v>
       </c>
@@ -2044,17 +1824,12 @@
       <c r="AL13" t="n">
         <v>0</v>
       </c>
-      <c r="AM13" t="inlineStr"/>
       <c r="AN13" t="n">
         <v>0</v>
       </c>
       <c r="AO13" t="n">
         <v>0</v>
       </c>
-      <c r="AP13" t="inlineStr"/>
-      <c r="AQ13" t="inlineStr"/>
-      <c r="AR13" t="inlineStr"/>
-      <c r="AS13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2109,8 +1884,6 @@
       <c r="L14" t="n">
         <v>10000000</v>
       </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -2119,17 +1892,6 @@
       <c r="P14" t="n">
         <v>0</v>
       </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="n">
         <v>0</v>
       </c>
@@ -2145,7 +1907,6 @@
       <c r="AF14" t="n">
         <v>0</v>
       </c>
-      <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="n">
         <v>0</v>
       </c>
@@ -2161,17 +1922,12 @@
       <c r="AL14" t="n">
         <v>0</v>
       </c>
-      <c r="AM14" t="inlineStr"/>
       <c r="AN14" t="n">
         <v>0</v>
       </c>
       <c r="AO14" t="n">
         <v>0</v>
       </c>
-      <c r="AP14" t="inlineStr"/>
-      <c r="AQ14" t="inlineStr"/>
-      <c r="AR14" t="inlineStr"/>
-      <c r="AS14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2226,8 +1982,6 @@
       <c r="L15" t="n">
         <v>5000000</v>
       </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -2236,17 +1990,6 @@
       <c r="P15" t="n">
         <v>0</v>
       </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="n">
         <v>0</v>
       </c>
@@ -2262,7 +2005,6 @@
       <c r="AF15" t="n">
         <v>0</v>
       </c>
-      <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="n">
         <v>0</v>
       </c>
@@ -2278,17 +2020,12 @@
       <c r="AL15" t="n">
         <v>0</v>
       </c>
-      <c r="AM15" t="inlineStr"/>
       <c r="AN15" t="n">
         <v>0</v>
       </c>
       <c r="AO15" t="n">
         <v>0</v>
       </c>
-      <c r="AP15" t="inlineStr"/>
-      <c r="AQ15" t="inlineStr"/>
-      <c r="AR15" t="inlineStr"/>
-      <c r="AS15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2343,8 +2080,6 @@
       <c r="L16" t="n">
         <v>5000000</v>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -2353,17 +2088,6 @@
       <c r="P16" t="n">
         <v>0</v>
       </c>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="n">
         <v>0</v>
       </c>
@@ -2379,7 +2103,6 @@
       <c r="AF16" t="n">
         <v>0</v>
       </c>
-      <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="n">
         <v>0</v>
       </c>
@@ -2395,17 +2118,12 @@
       <c r="AL16" t="n">
         <v>0</v>
       </c>
-      <c r="AM16" t="inlineStr"/>
       <c r="AN16" t="n">
         <v>0</v>
       </c>
       <c r="AO16" t="n">
         <v>0</v>
       </c>
-      <c r="AP16" t="inlineStr"/>
-      <c r="AQ16" t="inlineStr"/>
-      <c r="AR16" t="inlineStr"/>
-      <c r="AS16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2460,8 +2178,6 @@
       <c r="L17" t="n">
         <v>10000000</v>
       </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -2470,17 +2186,6 @@
       <c r="P17" t="n">
         <v>0</v>
       </c>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="n">
         <v>0</v>
       </c>
@@ -2496,7 +2201,6 @@
       <c r="AF17" t="n">
         <v>0</v>
       </c>
-      <c r="AG17" t="inlineStr"/>
       <c r="AH17" t="n">
         <v>0</v>
       </c>
@@ -2512,17 +2216,12 @@
       <c r="AL17" t="n">
         <v>0</v>
       </c>
-      <c r="AM17" t="inlineStr"/>
       <c r="AN17" t="n">
         <v>0</v>
       </c>
       <c r="AO17" t="n">
         <v>0</v>
       </c>
-      <c r="AP17" t="inlineStr"/>
-      <c r="AQ17" t="inlineStr"/>
-      <c r="AR17" t="inlineStr"/>
-      <c r="AS17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2577,8 +2276,6 @@
       <c r="L18" t="n">
         <v>10000000</v>
       </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -2587,17 +2284,6 @@
       <c r="P18" t="n">
         <v>0</v>
       </c>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
-      <c r="V18" t="inlineStr"/>
-      <c r="W18" t="inlineStr"/>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
-      <c r="Z18" t="inlineStr"/>
-      <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="n">
         <v>0</v>
       </c>
@@ -2613,7 +2299,6 @@
       <c r="AF18" t="n">
         <v>0</v>
       </c>
-      <c r="AG18" t="inlineStr"/>
       <c r="AH18" t="n">
         <v>0</v>
       </c>
@@ -2629,17 +2314,12 @@
       <c r="AL18" t="n">
         <v>0</v>
       </c>
-      <c r="AM18" t="inlineStr"/>
       <c r="AN18" t="n">
         <v>0</v>
       </c>
       <c r="AO18" t="n">
         <v>0</v>
       </c>
-      <c r="AP18" t="inlineStr"/>
-      <c r="AQ18" t="inlineStr"/>
-      <c r="AR18" t="inlineStr"/>
-      <c r="AS18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2694,8 +2374,6 @@
       <c r="L19" t="n">
         <v>10000000</v>
       </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -2704,17 +2382,6 @@
       <c r="P19" t="n">
         <v>0</v>
       </c>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
-      <c r="W19" t="inlineStr"/>
-      <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
-      <c r="Z19" t="inlineStr"/>
-      <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="n">
         <v>0</v>
       </c>
@@ -2730,7 +2397,6 @@
       <c r="AF19" t="n">
         <v>0</v>
       </c>
-      <c r="AG19" t="inlineStr"/>
       <c r="AH19" t="n">
         <v>0</v>
       </c>
@@ -2746,17 +2412,12 @@
       <c r="AL19" t="n">
         <v>0</v>
       </c>
-      <c r="AM19" t="inlineStr"/>
       <c r="AN19" t="n">
         <v>0</v>
       </c>
       <c r="AO19" t="n">
         <v>0</v>
       </c>
-      <c r="AP19" t="inlineStr"/>
-      <c r="AQ19" t="inlineStr"/>
-      <c r="AR19" t="inlineStr"/>
-      <c r="AS19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2811,8 +2472,6 @@
       <c r="L20" t="n">
         <v>10000000</v>
       </c>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -2821,17 +2480,6 @@
       <c r="P20" t="n">
         <v>0</v>
       </c>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
-      <c r="V20" t="inlineStr"/>
-      <c r="W20" t="inlineStr"/>
-      <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
-      <c r="Z20" t="inlineStr"/>
-      <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="n">
         <v>0</v>
       </c>
@@ -2847,7 +2495,6 @@
       <c r="AF20" t="n">
         <v>0</v>
       </c>
-      <c r="AG20" t="inlineStr"/>
       <c r="AH20" t="n">
         <v>0</v>
       </c>
@@ -2863,17 +2510,12 @@
       <c r="AL20" t="n">
         <v>0</v>
       </c>
-      <c r="AM20" t="inlineStr"/>
       <c r="AN20" t="n">
         <v>0</v>
       </c>
       <c r="AO20" t="n">
         <v>0</v>
       </c>
-      <c r="AP20" t="inlineStr"/>
-      <c r="AQ20" t="inlineStr"/>
-      <c r="AR20" t="inlineStr"/>
-      <c r="AS20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2928,8 +2570,6 @@
       <c r="L21" t="n">
         <v>10000000</v>
       </c>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -2938,17 +2578,6 @@
       <c r="P21" t="n">
         <v>0</v>
       </c>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
-      <c r="V21" t="inlineStr"/>
-      <c r="W21" t="inlineStr"/>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
-      <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="n">
         <v>0</v>
       </c>
@@ -2964,7 +2593,6 @@
       <c r="AF21" t="n">
         <v>0</v>
       </c>
-      <c r="AG21" t="inlineStr"/>
       <c r="AH21" t="n">
         <v>0</v>
       </c>
@@ -2980,17 +2608,12 @@
       <c r="AL21" t="n">
         <v>0</v>
       </c>
-      <c r="AM21" t="inlineStr"/>
       <c r="AN21" t="n">
         <v>0</v>
       </c>
       <c r="AO21" t="n">
         <v>0</v>
       </c>
-      <c r="AP21" t="inlineStr"/>
-      <c r="AQ21" t="inlineStr"/>
-      <c r="AR21" t="inlineStr"/>
-      <c r="AS21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3045,8 +2668,6 @@
       <c r="L22" t="n">
         <v>20000000</v>
       </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3055,17 +2676,6 @@
       <c r="P22" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
-      <c r="V22" t="inlineStr"/>
-      <c r="W22" t="inlineStr"/>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="inlineStr"/>
-      <c r="Z22" t="inlineStr"/>
-      <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="n">
         <v>0</v>
       </c>
@@ -3081,7 +2691,6 @@
       <c r="AF22" t="n">
         <v>0</v>
       </c>
-      <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="n">
         <v>0</v>
       </c>
@@ -3097,17 +2706,12 @@
       <c r="AL22" t="n">
         <v>0</v>
       </c>
-      <c r="AM22" t="inlineStr"/>
       <c r="AN22" t="n">
         <v>0</v>
       </c>
       <c r="AO22" t="n">
         <v>0</v>
       </c>
-      <c r="AP22" t="inlineStr"/>
-      <c r="AQ22" t="inlineStr"/>
-      <c r="AR22" t="inlineStr"/>
-      <c r="AS22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3125,7 +2729,6 @@
           <t>Maguindanao I</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
           <t>Tocao - Madidis National High School</t>
@@ -3160,8 +2763,6 @@
       <c r="L23" t="n">
         <v>20000000</v>
       </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3170,17 +2771,6 @@
       <c r="P23" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr"/>
-      <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="inlineStr"/>
-      <c r="Z23" t="inlineStr"/>
-      <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="n">
         <v>0</v>
       </c>
@@ -3196,7 +2786,6 @@
       <c r="AF23" t="n">
         <v>0</v>
       </c>
-      <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="n">
         <v>0</v>
       </c>
@@ -3212,17 +2801,12 @@
       <c r="AL23" t="n">
         <v>0</v>
       </c>
-      <c r="AM23" t="inlineStr"/>
       <c r="AN23" t="n">
         <v>0</v>
       </c>
       <c r="AO23" t="n">
         <v>0</v>
       </c>
-      <c r="AP23" t="inlineStr"/>
-      <c r="AQ23" t="inlineStr"/>
-      <c r="AR23" t="inlineStr"/>
-      <c r="AS23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3240,7 +2824,6 @@
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
           <t>Pura ES</t>
@@ -3275,8 +2858,6 @@
       <c r="L24" t="n">
         <v>5000000</v>
       </c>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3285,17 +2866,6 @@
       <c r="P24" t="n">
         <v>0</v>
       </c>
-      <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr"/>
-      <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
-      <c r="V24" t="inlineStr"/>
-      <c r="W24" t="inlineStr"/>
-      <c r="X24" t="inlineStr"/>
-      <c r="Y24" t="inlineStr"/>
-      <c r="Z24" t="inlineStr"/>
-      <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="n">
         <v>0</v>
       </c>
@@ -3311,7 +2881,6 @@
       <c r="AF24" t="n">
         <v>0</v>
       </c>
-      <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="n">
         <v>0</v>
       </c>
@@ -3327,17 +2896,12 @@
       <c r="AL24" t="n">
         <v>0</v>
       </c>
-      <c r="AM24" t="inlineStr"/>
       <c r="AN24" t="n">
         <v>0</v>
       </c>
       <c r="AO24" t="n">
         <v>0</v>
       </c>
-      <c r="AP24" t="inlineStr"/>
-      <c r="AQ24" t="inlineStr"/>
-      <c r="AR24" t="inlineStr"/>
-      <c r="AS24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3392,8 +2956,6 @@
       <c r="L25" t="n">
         <v>5000000</v>
       </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3402,17 +2964,6 @@
       <c r="P25" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
-      <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
-      <c r="W25" t="inlineStr"/>
-      <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="inlineStr"/>
-      <c r="Z25" t="inlineStr"/>
-      <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="n">
         <v>0</v>
       </c>
@@ -3428,7 +2979,6 @@
       <c r="AF25" t="n">
         <v>0</v>
       </c>
-      <c r="AG25" t="inlineStr"/>
       <c r="AH25" t="n">
         <v>0</v>
       </c>
@@ -3444,17 +2994,12 @@
       <c r="AL25" t="n">
         <v>0</v>
       </c>
-      <c r="AM25" t="inlineStr"/>
       <c r="AN25" t="n">
         <v>0</v>
       </c>
       <c r="AO25" t="n">
         <v>0</v>
       </c>
-      <c r="AP25" t="inlineStr"/>
-      <c r="AQ25" t="inlineStr"/>
-      <c r="AR25" t="inlineStr"/>
-      <c r="AS25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3509,8 +3054,6 @@
       <c r="L26" t="n">
         <v>5000000</v>
       </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3519,17 +3062,6 @@
       <c r="P26" t="n">
         <v>0</v>
       </c>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
-      <c r="V26" t="inlineStr"/>
-      <c r="W26" t="inlineStr"/>
-      <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="inlineStr"/>
-      <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="n">
         <v>0</v>
       </c>
@@ -3545,7 +3077,6 @@
       <c r="AF26" t="n">
         <v>0</v>
       </c>
-      <c r="AG26" t="inlineStr"/>
       <c r="AH26" t="n">
         <v>0</v>
       </c>
@@ -3561,17 +3092,12 @@
       <c r="AL26" t="n">
         <v>0</v>
       </c>
-      <c r="AM26" t="inlineStr"/>
       <c r="AN26" t="n">
         <v>0</v>
       </c>
       <c r="AO26" t="n">
         <v>0</v>
       </c>
-      <c r="AP26" t="inlineStr"/>
-      <c r="AQ26" t="inlineStr"/>
-      <c r="AR26" t="inlineStr"/>
-      <c r="AS26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3589,7 +3115,6 @@
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
           <t>Bayanga Norte ES</t>
@@ -3624,8 +3149,6 @@
       <c r="L27" t="n">
         <v>5000000</v>
       </c>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3634,17 +3157,6 @@
       <c r="P27" t="n">
         <v>0</v>
       </c>
-      <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
-      <c r="V27" t="inlineStr"/>
-      <c r="W27" t="inlineStr"/>
-      <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="inlineStr"/>
-      <c r="Z27" t="inlineStr"/>
-      <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="n">
         <v>0</v>
       </c>
@@ -3660,7 +3172,6 @@
       <c r="AF27" t="n">
         <v>0</v>
       </c>
-      <c r="AG27" t="inlineStr"/>
       <c r="AH27" t="n">
         <v>0</v>
       </c>
@@ -3676,17 +3187,12 @@
       <c r="AL27" t="n">
         <v>0</v>
       </c>
-      <c r="AM27" t="inlineStr"/>
       <c r="AN27" t="n">
         <v>0</v>
       </c>
       <c r="AO27" t="n">
         <v>0</v>
       </c>
-      <c r="AP27" t="inlineStr"/>
-      <c r="AQ27" t="inlineStr"/>
-      <c r="AR27" t="inlineStr"/>
-      <c r="AS27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3741,8 +3247,6 @@
       <c r="L28" t="n">
         <v>5000000</v>
       </c>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3751,17 +3255,6 @@
       <c r="P28" t="n">
         <v>0</v>
       </c>
-      <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
-      <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
-      <c r="V28" t="inlineStr"/>
-      <c r="W28" t="inlineStr"/>
-      <c r="X28" t="inlineStr"/>
-      <c r="Y28" t="inlineStr"/>
-      <c r="Z28" t="inlineStr"/>
-      <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="n">
         <v>0</v>
       </c>
@@ -3777,7 +3270,6 @@
       <c r="AF28" t="n">
         <v>0</v>
       </c>
-      <c r="AG28" t="inlineStr"/>
       <c r="AH28" t="n">
         <v>0</v>
       </c>
@@ -3793,17 +3285,12 @@
       <c r="AL28" t="n">
         <v>0</v>
       </c>
-      <c r="AM28" t="inlineStr"/>
       <c r="AN28" t="n">
         <v>0</v>
       </c>
       <c r="AO28" t="n">
         <v>0</v>
       </c>
-      <c r="AP28" t="inlineStr"/>
-      <c r="AQ28" t="inlineStr"/>
-      <c r="AR28" t="inlineStr"/>
-      <c r="AS28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3858,8 +3345,6 @@
       <c r="L29" t="n">
         <v>5000000</v>
       </c>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3868,17 +3353,6 @@
       <c r="P29" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
-      <c r="V29" t="inlineStr"/>
-      <c r="W29" t="inlineStr"/>
-      <c r="X29" t="inlineStr"/>
-      <c r="Y29" t="inlineStr"/>
-      <c r="Z29" t="inlineStr"/>
-      <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="n">
         <v>0</v>
       </c>
@@ -3894,7 +3368,6 @@
       <c r="AF29" t="n">
         <v>0</v>
       </c>
-      <c r="AG29" t="inlineStr"/>
       <c r="AH29" t="n">
         <v>0</v>
       </c>
@@ -3910,17 +3383,12 @@
       <c r="AL29" t="n">
         <v>0</v>
       </c>
-      <c r="AM29" t="inlineStr"/>
       <c r="AN29" t="n">
         <v>0</v>
       </c>
       <c r="AO29" t="n">
         <v>0</v>
       </c>
-      <c r="AP29" t="inlineStr"/>
-      <c r="AQ29" t="inlineStr"/>
-      <c r="AR29" t="inlineStr"/>
-      <c r="AS29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3938,7 +3406,6 @@
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
           <t>Inawan ES</t>
@@ -3973,8 +3440,6 @@
       <c r="L30" t="n">
         <v>5000000</v>
       </c>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3983,17 +3448,6 @@
       <c r="P30" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
-      <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
-      <c r="V30" t="inlineStr"/>
-      <c r="W30" t="inlineStr"/>
-      <c r="X30" t="inlineStr"/>
-      <c r="Y30" t="inlineStr"/>
-      <c r="Z30" t="inlineStr"/>
-      <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="n">
         <v>0</v>
       </c>
@@ -4009,7 +3463,6 @@
       <c r="AF30" t="n">
         <v>0</v>
       </c>
-      <c r="AG30" t="inlineStr"/>
       <c r="AH30" t="n">
         <v>0</v>
       </c>
@@ -4025,17 +3478,12 @@
       <c r="AL30" t="n">
         <v>0</v>
       </c>
-      <c r="AM30" t="inlineStr"/>
       <c r="AN30" t="n">
         <v>0</v>
       </c>
       <c r="AO30" t="n">
         <v>0</v>
       </c>
-      <c r="AP30" t="inlineStr"/>
-      <c r="AQ30" t="inlineStr"/>
-      <c r="AR30" t="inlineStr"/>
-      <c r="AS30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4090,8 +3538,6 @@
       <c r="L31" t="n">
         <v>5000000</v>
       </c>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -4100,17 +3546,6 @@
       <c r="P31" t="n">
         <v>0</v>
       </c>
-      <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr"/>
-      <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr"/>
-      <c r="V31" t="inlineStr"/>
-      <c r="W31" t="inlineStr"/>
-      <c r="X31" t="inlineStr"/>
-      <c r="Y31" t="inlineStr"/>
-      <c r="Z31" t="inlineStr"/>
-      <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="n">
         <v>0</v>
       </c>
@@ -4126,7 +3561,6 @@
       <c r="AF31" t="n">
         <v>0</v>
       </c>
-      <c r="AG31" t="inlineStr"/>
       <c r="AH31" t="n">
         <v>0</v>
       </c>
@@ -4142,17 +3576,12 @@
       <c r="AL31" t="n">
         <v>0</v>
       </c>
-      <c r="AM31" t="inlineStr"/>
       <c r="AN31" t="n">
         <v>0</v>
       </c>
       <c r="AO31" t="n">
         <v>0</v>
       </c>
-      <c r="AP31" t="inlineStr"/>
-      <c r="AQ31" t="inlineStr"/>
-      <c r="AR31" t="inlineStr"/>
-      <c r="AS31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4207,8 +3636,6 @@
       <c r="L32" t="n">
         <v>42000000</v>
       </c>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -4217,17 +3644,6 @@
       <c r="P32" t="n">
         <v>0</v>
       </c>
-      <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
-      <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr"/>
-      <c r="V32" t="inlineStr"/>
-      <c r="W32" t="inlineStr"/>
-      <c r="X32" t="inlineStr"/>
-      <c r="Y32" t="inlineStr"/>
-      <c r="Z32" t="inlineStr"/>
-      <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="n">
         <v>0</v>
       </c>
@@ -4243,7 +3659,6 @@
       <c r="AF32" t="n">
         <v>0</v>
       </c>
-      <c r="AG32" t="inlineStr"/>
       <c r="AH32" t="n">
         <v>0</v>
       </c>
@@ -4259,17 +3674,12 @@
       <c r="AL32" t="n">
         <v>0</v>
       </c>
-      <c r="AM32" t="inlineStr"/>
       <c r="AN32" t="n">
         <v>0</v>
       </c>
       <c r="AO32" t="n">
         <v>0</v>
       </c>
-      <c r="AP32" t="inlineStr"/>
-      <c r="AQ32" t="inlineStr"/>
-      <c r="AR32" t="inlineStr"/>
-      <c r="AS32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4324,8 +3734,6 @@
       <c r="L33" t="n">
         <v>10000000</v>
       </c>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -4334,17 +3742,6 @@
       <c r="P33" t="n">
         <v>0</v>
       </c>
-      <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
-      <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
-      <c r="V33" t="inlineStr"/>
-      <c r="W33" t="inlineStr"/>
-      <c r="X33" t="inlineStr"/>
-      <c r="Y33" t="inlineStr"/>
-      <c r="Z33" t="inlineStr"/>
-      <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="n">
         <v>0</v>
       </c>
@@ -4360,7 +3757,6 @@
       <c r="AF33" t="n">
         <v>0</v>
       </c>
-      <c r="AG33" t="inlineStr"/>
       <c r="AH33" t="n">
         <v>0</v>
       </c>
@@ -4376,17 +3772,12 @@
       <c r="AL33" t="n">
         <v>0</v>
       </c>
-      <c r="AM33" t="inlineStr"/>
       <c r="AN33" t="n">
         <v>0</v>
       </c>
       <c r="AO33" t="n">
         <v>0</v>
       </c>
-      <c r="AP33" t="inlineStr"/>
-      <c r="AQ33" t="inlineStr"/>
-      <c r="AR33" t="inlineStr"/>
-      <c r="AS33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4404,7 +3795,6 @@
           <t>Sulu</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
           <t>Sultan Jamalul Kiram Central High School</t>
@@ -4439,8 +3829,6 @@
       <c r="L34" t="n">
         <v>40000000</v>
       </c>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -4449,17 +3837,6 @@
       <c r="P34" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr"/>
-      <c r="S34" t="inlineStr"/>
-      <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr"/>
-      <c r="V34" t="inlineStr"/>
-      <c r="W34" t="inlineStr"/>
-      <c r="X34" t="inlineStr"/>
-      <c r="Y34" t="inlineStr"/>
-      <c r="Z34" t="inlineStr"/>
-      <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="n">
         <v>0</v>
       </c>
@@ -4475,7 +3852,6 @@
       <c r="AF34" t="n">
         <v>0</v>
       </c>
-      <c r="AG34" t="inlineStr"/>
       <c r="AH34" t="n">
         <v>0</v>
       </c>
@@ -4491,17 +3867,12 @@
       <c r="AL34" t="n">
         <v>0</v>
       </c>
-      <c r="AM34" t="inlineStr"/>
       <c r="AN34" t="n">
         <v>0</v>
       </c>
       <c r="AO34" t="n">
         <v>0</v>
       </c>
-      <c r="AP34" t="inlineStr"/>
-      <c r="AQ34" t="inlineStr"/>
-      <c r="AR34" t="inlineStr"/>
-      <c r="AS34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4519,7 +3890,6 @@
           <t>Sulu</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
           <t>Patikul NHS - Extension</t>
@@ -4554,8 +3924,6 @@
       <c r="L35" t="n">
         <v>10000000</v>
       </c>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -4564,17 +3932,6 @@
       <c r="P35" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
-      <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
-      <c r="V35" t="inlineStr"/>
-      <c r="W35" t="inlineStr"/>
-      <c r="X35" t="inlineStr"/>
-      <c r="Y35" t="inlineStr"/>
-      <c r="Z35" t="inlineStr"/>
-      <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="n">
         <v>0</v>
       </c>
@@ -4590,7 +3947,6 @@
       <c r="AF35" t="n">
         <v>0</v>
       </c>
-      <c r="AG35" t="inlineStr"/>
       <c r="AH35" t="n">
         <v>0</v>
       </c>
@@ -4606,17 +3962,12 @@
       <c r="AL35" t="n">
         <v>0</v>
       </c>
-      <c r="AM35" t="inlineStr"/>
       <c r="AN35" t="n">
         <v>0</v>
       </c>
       <c r="AO35" t="n">
         <v>0</v>
       </c>
-      <c r="AP35" t="inlineStr"/>
-      <c r="AQ35" t="inlineStr"/>
-      <c r="AR35" t="inlineStr"/>
-      <c r="AS35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4671,8 +4022,6 @@
       <c r="L36" t="n">
         <v>40000000</v>
       </c>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -4681,17 +4030,6 @@
       <c r="P36" t="n">
         <v>0</v>
       </c>
-      <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
-      <c r="S36" t="inlineStr"/>
-      <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
-      <c r="V36" t="inlineStr"/>
-      <c r="W36" t="inlineStr"/>
-      <c r="X36" t="inlineStr"/>
-      <c r="Y36" t="inlineStr"/>
-      <c r="Z36" t="inlineStr"/>
-      <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="n">
         <v>0</v>
       </c>
@@ -4707,7 +4045,6 @@
       <c r="AF36" t="n">
         <v>0</v>
       </c>
-      <c r="AG36" t="inlineStr"/>
       <c r="AH36" t="n">
         <v>0</v>
       </c>
@@ -4723,17 +4060,12 @@
       <c r="AL36" t="n">
         <v>0</v>
       </c>
-      <c r="AM36" t="inlineStr"/>
       <c r="AN36" t="n">
         <v>0</v>
       </c>
       <c r="AO36" t="n">
         <v>0</v>
       </c>
-      <c r="AP36" t="inlineStr"/>
-      <c r="AQ36" t="inlineStr"/>
-      <c r="AR36" t="inlineStr"/>
-      <c r="AS36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4788,8 +4120,6 @@
       <c r="L37" t="n">
         <v>7329687.55</v>
       </c>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -4798,17 +4128,6 @@
       <c r="P37" t="n">
         <v>0</v>
       </c>
-      <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
-      <c r="S37" t="inlineStr"/>
-      <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
-      <c r="V37" t="inlineStr"/>
-      <c r="W37" t="inlineStr"/>
-      <c r="X37" t="inlineStr"/>
-      <c r="Y37" t="inlineStr"/>
-      <c r="Z37" t="inlineStr"/>
-      <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="n">
         <v>0</v>
       </c>
@@ -4824,7 +4143,6 @@
       <c r="AF37" t="n">
         <v>0</v>
       </c>
-      <c r="AG37" t="inlineStr"/>
       <c r="AH37" t="n">
         <v>0</v>
       </c>
@@ -4840,17 +4158,12 @@
       <c r="AL37" t="n">
         <v>0</v>
       </c>
-      <c r="AM37" t="inlineStr"/>
       <c r="AN37" t="n">
         <v>0</v>
       </c>
       <c r="AO37" t="n">
         <v>0</v>
       </c>
-      <c r="AP37" t="inlineStr"/>
-      <c r="AQ37" t="inlineStr"/>
-      <c r="AR37" t="inlineStr"/>
-      <c r="AS37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4905,8 +4218,6 @@
       <c r="L38" t="n">
         <v>7329687.55</v>
       </c>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -4915,17 +4226,6 @@
       <c r="P38" t="n">
         <v>0</v>
       </c>
-      <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr"/>
-      <c r="S38" t="inlineStr"/>
-      <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
-      <c r="V38" t="inlineStr"/>
-      <c r="W38" t="inlineStr"/>
-      <c r="X38" t="inlineStr"/>
-      <c r="Y38" t="inlineStr"/>
-      <c r="Z38" t="inlineStr"/>
-      <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="n">
         <v>0</v>
       </c>
@@ -4941,7 +4241,6 @@
       <c r="AF38" t="n">
         <v>0</v>
       </c>
-      <c r="AG38" t="inlineStr"/>
       <c r="AH38" t="n">
         <v>0</v>
       </c>
@@ -4957,17 +4256,12 @@
       <c r="AL38" t="n">
         <v>0</v>
       </c>
-      <c r="AM38" t="inlineStr"/>
       <c r="AN38" t="n">
         <v>0</v>
       </c>
       <c r="AO38" t="n">
         <v>0</v>
       </c>
-      <c r="AP38" t="inlineStr"/>
-      <c r="AQ38" t="inlineStr"/>
-      <c r="AR38" t="inlineStr"/>
-      <c r="AS38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5022,8 +4316,6 @@
       <c r="L39" t="n">
         <v>5670312.45</v>
       </c>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -5032,17 +4324,6 @@
       <c r="P39" t="n">
         <v>0</v>
       </c>
-      <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr"/>
-      <c r="S39" t="inlineStr"/>
-      <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
-      <c r="V39" t="inlineStr"/>
-      <c r="W39" t="inlineStr"/>
-      <c r="X39" t="inlineStr"/>
-      <c r="Y39" t="inlineStr"/>
-      <c r="Z39" t="inlineStr"/>
-      <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="n">
         <v>0</v>
       </c>
@@ -5058,7 +4339,6 @@
       <c r="AF39" t="n">
         <v>0</v>
       </c>
-      <c r="AG39" t="inlineStr"/>
       <c r="AH39" t="n">
         <v>0</v>
       </c>
@@ -5074,17 +4354,12 @@
       <c r="AL39" t="n">
         <v>0</v>
       </c>
-      <c r="AM39" t="inlineStr"/>
       <c r="AN39" t="n">
         <v>0</v>
       </c>
       <c r="AO39" t="n">
         <v>0</v>
       </c>
-      <c r="AP39" t="inlineStr"/>
-      <c r="AQ39" t="inlineStr"/>
-      <c r="AR39" t="inlineStr"/>
-      <c r="AS39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5139,8 +4414,6 @@
       <c r="L40" t="n">
         <v>5670312.45</v>
       </c>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -5149,17 +4422,6 @@
       <c r="P40" t="n">
         <v>0</v>
       </c>
-      <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr"/>
-      <c r="S40" t="inlineStr"/>
-      <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
-      <c r="V40" t="inlineStr"/>
-      <c r="W40" t="inlineStr"/>
-      <c r="X40" t="inlineStr"/>
-      <c r="Y40" t="inlineStr"/>
-      <c r="Z40" t="inlineStr"/>
-      <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="n">
         <v>0</v>
       </c>
@@ -5175,7 +4437,6 @@
       <c r="AF40" t="n">
         <v>0</v>
       </c>
-      <c r="AG40" t="inlineStr"/>
       <c r="AH40" t="n">
         <v>0</v>
       </c>
@@ -5191,17 +4452,12 @@
       <c r="AL40" t="n">
         <v>0</v>
       </c>
-      <c r="AM40" t="inlineStr"/>
       <c r="AN40" t="n">
         <v>0</v>
       </c>
       <c r="AO40" t="n">
         <v>0</v>
       </c>
-      <c r="AP40" t="inlineStr"/>
-      <c r="AQ40" t="inlineStr"/>
-      <c r="AR40" t="inlineStr"/>
-      <c r="AS40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5256,8 +4512,6 @@
       <c r="L41" t="n">
         <v>5000000</v>
       </c>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5266,17 +4520,6 @@
       <c r="P41" t="n">
         <v>0</v>
       </c>
-      <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
-      <c r="S41" t="inlineStr"/>
-      <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
-      <c r="V41" t="inlineStr"/>
-      <c r="W41" t="inlineStr"/>
-      <c r="X41" t="inlineStr"/>
-      <c r="Y41" t="inlineStr"/>
-      <c r="Z41" t="inlineStr"/>
-      <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="n">
         <v>0</v>
       </c>
@@ -5292,7 +4535,6 @@
       <c r="AF41" t="n">
         <v>0</v>
       </c>
-      <c r="AG41" t="inlineStr"/>
       <c r="AH41" t="n">
         <v>0</v>
       </c>
@@ -5308,17 +4550,12 @@
       <c r="AL41" t="n">
         <v>0</v>
       </c>
-      <c r="AM41" t="inlineStr"/>
       <c r="AN41" t="n">
         <v>0</v>
       </c>
       <c r="AO41" t="n">
         <v>0</v>
       </c>
-      <c r="AP41" t="inlineStr"/>
-      <c r="AQ41" t="inlineStr"/>
-      <c r="AR41" t="inlineStr"/>
-      <c r="AS41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5373,8 +4610,6 @@
       <c r="L42" t="n">
         <v>5000000</v>
       </c>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5383,17 +4618,6 @@
       <c r="P42" t="n">
         <v>0</v>
       </c>
-      <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr"/>
-      <c r="S42" t="inlineStr"/>
-      <c r="T42" t="inlineStr"/>
-      <c r="U42" t="inlineStr"/>
-      <c r="V42" t="inlineStr"/>
-      <c r="W42" t="inlineStr"/>
-      <c r="X42" t="inlineStr"/>
-      <c r="Y42" t="inlineStr"/>
-      <c r="Z42" t="inlineStr"/>
-      <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="n">
         <v>0</v>
       </c>
@@ -5409,7 +4633,6 @@
       <c r="AF42" t="n">
         <v>0</v>
       </c>
-      <c r="AG42" t="inlineStr"/>
       <c r="AH42" t="n">
         <v>0</v>
       </c>
@@ -5425,17 +4648,12 @@
       <c r="AL42" t="n">
         <v>0</v>
       </c>
-      <c r="AM42" t="inlineStr"/>
       <c r="AN42" t="n">
         <v>0</v>
       </c>
       <c r="AO42" t="n">
         <v>0</v>
       </c>
-      <c r="AP42" t="inlineStr"/>
-      <c r="AQ42" t="inlineStr"/>
-      <c r="AR42" t="inlineStr"/>
-      <c r="AS42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5490,8 +4708,6 @@
       <c r="L43" t="n">
         <v>5000000</v>
       </c>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5500,17 +4716,6 @@
       <c r="P43" t="n">
         <v>0</v>
       </c>
-      <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr"/>
-      <c r="S43" t="inlineStr"/>
-      <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
-      <c r="V43" t="inlineStr"/>
-      <c r="W43" t="inlineStr"/>
-      <c r="X43" t="inlineStr"/>
-      <c r="Y43" t="inlineStr"/>
-      <c r="Z43" t="inlineStr"/>
-      <c r="AA43" t="inlineStr"/>
       <c r="AB43" t="n">
         <v>0</v>
       </c>
@@ -5526,7 +4731,6 @@
       <c r="AF43" t="n">
         <v>0</v>
       </c>
-      <c r="AG43" t="inlineStr"/>
       <c r="AH43" t="n">
         <v>0</v>
       </c>
@@ -5542,17 +4746,12 @@
       <c r="AL43" t="n">
         <v>0</v>
       </c>
-      <c r="AM43" t="inlineStr"/>
       <c r="AN43" t="n">
         <v>0</v>
       </c>
       <c r="AO43" t="n">
         <v>0</v>
       </c>
-      <c r="AP43" t="inlineStr"/>
-      <c r="AQ43" t="inlineStr"/>
-      <c r="AR43" t="inlineStr"/>
-      <c r="AS43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5570,7 +4769,6 @@
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
           <t>Lupah Pula CS</t>
@@ -5605,8 +4803,6 @@
       <c r="L44" t="n">
         <v>5000000</v>
       </c>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5615,17 +4811,6 @@
       <c r="P44" t="n">
         <v>0</v>
       </c>
-      <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
-      <c r="S44" t="inlineStr"/>
-      <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr"/>
-      <c r="V44" t="inlineStr"/>
-      <c r="W44" t="inlineStr"/>
-      <c r="X44" t="inlineStr"/>
-      <c r="Y44" t="inlineStr"/>
-      <c r="Z44" t="inlineStr"/>
-      <c r="AA44" t="inlineStr"/>
       <c r="AB44" t="n">
         <v>0</v>
       </c>
@@ -5641,7 +4826,6 @@
       <c r="AF44" t="n">
         <v>0</v>
       </c>
-      <c r="AG44" t="inlineStr"/>
       <c r="AH44" t="n">
         <v>0</v>
       </c>
@@ -5657,17 +4841,12 @@
       <c r="AL44" t="n">
         <v>0</v>
       </c>
-      <c r="AM44" t="inlineStr"/>
       <c r="AN44" t="n">
         <v>0</v>
       </c>
       <c r="AO44" t="n">
         <v>0</v>
       </c>
-      <c r="AP44" t="inlineStr"/>
-      <c r="AQ44" t="inlineStr"/>
-      <c r="AR44" t="inlineStr"/>
-      <c r="AS44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5722,8 +4901,6 @@
       <c r="L45" t="n">
         <v>5000000</v>
       </c>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5732,17 +4909,6 @@
       <c r="P45" t="n">
         <v>0</v>
       </c>
-      <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
-      <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr"/>
-      <c r="V45" t="inlineStr"/>
-      <c r="W45" t="inlineStr"/>
-      <c r="X45" t="inlineStr"/>
-      <c r="Y45" t="inlineStr"/>
-      <c r="Z45" t="inlineStr"/>
-      <c r="AA45" t="inlineStr"/>
       <c r="AB45" t="n">
         <v>0</v>
       </c>
@@ -5758,7 +4924,6 @@
       <c r="AF45" t="n">
         <v>0</v>
       </c>
-      <c r="AG45" t="inlineStr"/>
       <c r="AH45" t="n">
         <v>0</v>
       </c>
@@ -5774,17 +4939,12 @@
       <c r="AL45" t="n">
         <v>0</v>
       </c>
-      <c r="AM45" t="inlineStr"/>
       <c r="AN45" t="n">
         <v>0</v>
       </c>
       <c r="AO45" t="n">
         <v>0</v>
       </c>
-      <c r="AP45" t="inlineStr"/>
-      <c r="AQ45" t="inlineStr"/>
-      <c r="AR45" t="inlineStr"/>
-      <c r="AS45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5839,8 +4999,6 @@
       <c r="L46" t="n">
         <v>5000000</v>
       </c>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5849,17 +5007,6 @@
       <c r="P46" t="n">
         <v>0</v>
       </c>
-      <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr"/>
-      <c r="S46" t="inlineStr"/>
-      <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr"/>
-      <c r="W46" t="inlineStr"/>
-      <c r="X46" t="inlineStr"/>
-      <c r="Y46" t="inlineStr"/>
-      <c r="Z46" t="inlineStr"/>
-      <c r="AA46" t="inlineStr"/>
       <c r="AB46" t="n">
         <v>0</v>
       </c>
@@ -5875,7 +5022,6 @@
       <c r="AF46" t="n">
         <v>0</v>
       </c>
-      <c r="AG46" t="inlineStr"/>
       <c r="AH46" t="n">
         <v>0</v>
       </c>
@@ -5891,17 +5037,12 @@
       <c r="AL46" t="n">
         <v>0</v>
       </c>
-      <c r="AM46" t="inlineStr"/>
       <c r="AN46" t="n">
         <v>0</v>
       </c>
       <c r="AO46" t="n">
         <v>0</v>
       </c>
-      <c r="AP46" t="inlineStr"/>
-      <c r="AQ46" t="inlineStr"/>
-      <c r="AR46" t="inlineStr"/>
-      <c r="AS46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5956,8 +5097,6 @@
       <c r="L47" t="n">
         <v>5000000</v>
       </c>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5966,17 +5105,6 @@
       <c r="P47" t="n">
         <v>0</v>
       </c>
-      <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
-      <c r="S47" t="inlineStr"/>
-      <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
-      <c r="V47" t="inlineStr"/>
-      <c r="W47" t="inlineStr"/>
-      <c r="X47" t="inlineStr"/>
-      <c r="Y47" t="inlineStr"/>
-      <c r="Z47" t="inlineStr"/>
-      <c r="AA47" t="inlineStr"/>
       <c r="AB47" t="n">
         <v>0</v>
       </c>
@@ -5992,7 +5120,6 @@
       <c r="AF47" t="n">
         <v>0</v>
       </c>
-      <c r="AG47" t="inlineStr"/>
       <c r="AH47" t="n">
         <v>0</v>
       </c>
@@ -6008,17 +5135,12 @@
       <c r="AL47" t="n">
         <v>0</v>
       </c>
-      <c r="AM47" t="inlineStr"/>
       <c r="AN47" t="n">
         <v>0</v>
       </c>
       <c r="AO47" t="n">
         <v>0</v>
       </c>
-      <c r="AP47" t="inlineStr"/>
-      <c r="AQ47" t="inlineStr"/>
-      <c r="AR47" t="inlineStr"/>
-      <c r="AS47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6036,7 +5158,6 @@
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
           <t>Tabawan Stand Alone Senior High School</t>
@@ -6071,8 +5192,6 @@
       <c r="L48" t="n">
         <v>5000000</v>
       </c>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -6081,17 +5200,6 @@
       <c r="P48" t="n">
         <v>0</v>
       </c>
-      <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr"/>
-      <c r="S48" t="inlineStr"/>
-      <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr"/>
-      <c r="V48" t="inlineStr"/>
-      <c r="W48" t="inlineStr"/>
-      <c r="X48" t="inlineStr"/>
-      <c r="Y48" t="inlineStr"/>
-      <c r="Z48" t="inlineStr"/>
-      <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="n">
         <v>0</v>
       </c>
@@ -6107,7 +5215,6 @@
       <c r="AF48" t="n">
         <v>0</v>
       </c>
-      <c r="AG48" t="inlineStr"/>
       <c r="AH48" t="n">
         <v>0</v>
       </c>
@@ -6123,17 +5230,85 @@
       <c r="AL48" t="n">
         <v>0</v>
       </c>
-      <c r="AM48" t="inlineStr"/>
       <c r="AN48" t="n">
         <v>0</v>
       </c>
       <c r="AO48" t="n">
         <v>0</v>
       </c>
-      <c r="AP48" t="inlineStr"/>
-      <c r="AQ48" t="inlineStr"/>
-      <c r="AR48" t="inlineStr"/>
-      <c r="AS48" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="AT2:AT48" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=DropdownOptions!$A$1:$A$7</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>0% - 10%: Foundation completed: Groundwork finished; no vertical structure yet.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>11% - 25%: Structure and rough-in started: Structural framing in progress; initial MEP rough-in.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>26% - 50%: Structure erected, partial roofing: Building shape defined; roof and systems advancing.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>51% - 75%: Exterior sealed, interior work underway: Enclosed structure; painting, flooring, and testing begin.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">76% - 90%: Final finishes and inspections: Systems tested; </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>91% - 99%: Final touches and punch list: Minor adjustments; final inspections and approvals.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>100% - Construction complete: Ready for handover and occupancy.</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Used most updated status accomplishmnet files as of may
</commit_message>
<xml_diff>
--- a/Filtered_By_Region/BARMM/BARMM_NEWCON.xlsx
+++ b/Filtered_By_Region/BARMM/BARMM_NEWCON.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AT48"/>
+  <dimension ref="A1:AC48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,7 +477,8 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>No. of Classrooms</t>
+          <t>PHYSICAL TARGET
+(# OF CL)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -572,106 +573,16 @@
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>No. of Sites Reverted</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>No. of Sites Not yet started</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>No. of Sites Under Procurement</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>No. of Sites On Going</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>No. of Sites Completed</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>No. of Sites Terminated</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>No. of CL Reverted</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>No. of CL Not yet started</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>No. of CL Under Procurement</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>No. of CL On Going</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>No. of CL Completed</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>No. of CL Terminated</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>Previous %</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>Difference</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>STOREY</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>No. of Sites (original)</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>No. of Classrooms (original)</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>Project Allocation (original)</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
+          <t>Program-Year</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
         <is>
           <t>Status as of July 4, 2025</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -695,11 +606,6 @@
           <t>CITY OF ISABELA (Capital)</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
@@ -724,49 +630,13 @@
       <c r="P2" t="n">
         <v>0</v>
       </c>
-      <c r="AB2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0</v>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -790,11 +660,6 @@
           <t>CITY OF LAMITAN</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
@@ -822,49 +687,13 @@
       <c r="P3" t="n">
         <v>0</v>
       </c>
-      <c r="AB3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>16</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>0</v>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -883,11 +712,6 @@
           <t>BUMBARAN</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H4" t="n">
         <v>1</v>
       </c>
@@ -915,49 +739,13 @@
       <c r="P4" t="n">
         <v>0</v>
       </c>
-      <c r="AB4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>0</v>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -981,11 +769,6 @@
           <t>BUMBARAN</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
@@ -1013,49 +796,13 @@
       <c r="P5" t="n">
         <v>0</v>
       </c>
-      <c r="AB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>0</v>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -1079,11 +826,6 @@
           <t>DITSAAN-RAMAIN</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H6" t="n">
         <v>1</v>
       </c>
@@ -1105,55 +847,19 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P6" t="n">
         <v>0</v>
       </c>
-      <c r="AB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>0</v>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -1177,11 +883,6 @@
           <t>MARANTAO</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H7" t="n">
         <v>1</v>
       </c>
@@ -1203,55 +904,19 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P7" t="n">
         <v>0</v>
       </c>
-      <c r="AB7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>0</v>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -1275,11 +940,6 @@
           <t>POONA BAYABAO (GATA)</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
@@ -1307,49 +967,13 @@
       <c r="P8" t="n">
         <v>0</v>
       </c>
-      <c r="AB8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>0</v>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -1373,11 +997,6 @@
           <t>WAO</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H9" t="n">
         <v>1</v>
       </c>
@@ -1399,55 +1018,19 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P9" t="n">
         <v>0</v>
       </c>
-      <c r="AB9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO9" t="n">
-        <v>0</v>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -1471,11 +1054,6 @@
           <t>WAO</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
@@ -1503,49 +1081,13 @@
       <c r="P10" t="n">
         <v>0</v>
       </c>
-      <c r="AB10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI10" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO10" t="n">
-        <v>0</v>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -1569,11 +1111,6 @@
           <t>MADALUM</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
@@ -1601,49 +1138,13 @@
       <c r="P11" t="n">
         <v>0</v>
       </c>
-      <c r="AB11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI11" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO11" t="n">
-        <v>0</v>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -1667,11 +1168,6 @@
           <t>MADAMBA</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H12" t="n">
         <v>1</v>
       </c>
@@ -1699,49 +1195,13 @@
       <c r="P12" t="n">
         <v>0</v>
       </c>
-      <c r="AB12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI12" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO12" t="n">
-        <v>0</v>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -1760,11 +1220,6 @@
       <c r="F13" t="inlineStr">
         <is>
           <t>MADAMBA</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2nd</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -1794,49 +1249,13 @@
       <c r="P13" t="n">
         <v>0</v>
       </c>
-      <c r="AB13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI13" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO13" t="n">
-        <v>0</v>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -1860,11 +1279,6 @@
           <t>MALABANG</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
@@ -1892,49 +1306,13 @@
       <c r="P14" t="n">
         <v>0</v>
       </c>
-      <c r="AB14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO14" t="n">
-        <v>0</v>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -1958,11 +1336,6 @@
           <t>SULTAN GUMANDER (PICONG)</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H15" t="n">
         <v>1</v>
       </c>
@@ -1990,49 +1363,13 @@
       <c r="P15" t="n">
         <v>0</v>
       </c>
-      <c r="AB15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI15" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO15" t="n">
-        <v>0</v>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -2056,11 +1393,6 @@
           <t>TUGAYA</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H16" t="n">
         <v>1</v>
       </c>
@@ -2088,49 +1420,13 @@
       <c r="P16" t="n">
         <v>0</v>
       </c>
-      <c r="AB16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI16" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO16" t="n">
-        <v>0</v>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -2154,11 +1450,6 @@
           <t>AMPATUAN</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H17" t="n">
         <v>1</v>
       </c>
@@ -2180,55 +1471,19 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P17" t="n">
         <v>0</v>
       </c>
-      <c r="AB17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO17" t="n">
-        <v>0</v>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -2252,11 +1507,6 @@
           <t>BULUAN</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H18" t="n">
         <v>1</v>
       </c>
@@ -2278,55 +1528,19 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P18" t="n">
         <v>0</v>
       </c>
-      <c r="AB18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO18" t="n">
-        <v>0</v>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -2350,11 +1564,6 @@
           <t>DATU MONTAWAL (PAGAGAWAN)</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H19" t="n">
         <v>1</v>
       </c>
@@ -2376,55 +1585,19 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P19" t="n">
         <v>0</v>
       </c>
-      <c r="AB19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO19" t="n">
-        <v>0</v>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B20" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -2448,11 +1621,6 @@
           <t>PAGALUNGAN</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H20" t="n">
         <v>1</v>
       </c>
@@ -2474,55 +1642,19 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P20" t="n">
         <v>0</v>
       </c>
-      <c r="AB20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO20" t="n">
-        <v>0</v>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -2546,11 +1678,6 @@
           <t>SOUTH UPI</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H21" t="n">
         <v>1</v>
       </c>
@@ -2572,55 +1699,19 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P21" t="n">
         <v>0</v>
       </c>
-      <c r="AB21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO21" t="n">
-        <v>0</v>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B22" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -2644,11 +1735,6 @@
           <t>DATU PAGLAS</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H22" t="n">
         <v>1</v>
       </c>
@@ -2676,49 +1762,13 @@
       <c r="P22" t="n">
         <v>0</v>
       </c>
-      <c r="AB22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI22" t="n">
-        <v>8</v>
-      </c>
-      <c r="AJ22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO22" t="n">
-        <v>0</v>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -2737,11 +1787,6 @@
       <c r="F23" t="inlineStr">
         <is>
           <t>DATU PAGLAS</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2nd</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -2771,49 +1816,13 @@
       <c r="P23" t="n">
         <v>0</v>
       </c>
-      <c r="AB23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI23" t="n">
-        <v>8</v>
-      </c>
-      <c r="AJ23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO23" t="n">
-        <v>0</v>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -2832,11 +1841,6 @@
       <c r="F24" t="inlineStr">
         <is>
           <t>DATU BLAH T. SINSUAT</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>1st</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -2866,49 +1870,13 @@
       <c r="P24" t="n">
         <v>0</v>
       </c>
-      <c r="AB24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC24" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI24" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO24" t="n">
-        <v>0</v>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B25" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -2932,11 +1900,6 @@
           <t>KABUNTALAN (TUMBAO)</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H25" t="n">
         <v>1</v>
       </c>
@@ -2964,49 +1927,13 @@
       <c r="P25" t="n">
         <v>0</v>
       </c>
-      <c r="AB25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC25" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI25" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO25" t="n">
-        <v>0</v>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B26" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3030,11 +1957,6 @@
           <t>KABUNTALAN (TUMBAO)</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H26" t="n">
         <v>1</v>
       </c>
@@ -3062,49 +1984,13 @@
       <c r="P26" t="n">
         <v>0</v>
       </c>
-      <c r="AB26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC26" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI26" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO26" t="n">
-        <v>0</v>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B27" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3123,11 +2009,6 @@
       <c r="F27" t="inlineStr">
         <is>
           <t>MATANOG</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>1st</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -3157,49 +2038,13 @@
       <c r="P27" t="n">
         <v>0</v>
       </c>
-      <c r="AB27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC27" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI27" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO27" t="n">
-        <v>0</v>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B28" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3223,11 +2068,6 @@
           <t>SULTAN KUDARAT (NULING)</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H28" t="n">
         <v>1</v>
       </c>
@@ -3255,49 +2095,13 @@
       <c r="P28" t="n">
         <v>0</v>
       </c>
-      <c r="AB28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC28" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI28" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO28" t="n">
-        <v>0</v>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B29" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3321,11 +2125,6 @@
           <t>SULTAN KUDARAT (NULING)</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H29" t="n">
         <v>1</v>
       </c>
@@ -3353,49 +2152,13 @@
       <c r="P29" t="n">
         <v>0</v>
       </c>
-      <c r="AB29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC29" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI29" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO29" t="n">
-        <v>0</v>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B30" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3414,11 +2177,6 @@
       <c r="F30" t="inlineStr">
         <is>
           <t>SULTAN KUDARAT (NULING)</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>1st</t>
         </is>
       </c>
       <c r="H30" t="n">
@@ -3448,49 +2206,13 @@
       <c r="P30" t="n">
         <v>0</v>
       </c>
-      <c r="AB30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC30" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI30" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO30" t="n">
-        <v>0</v>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B31" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3514,11 +2236,6 @@
           <t>UPI</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H31" t="n">
         <v>1</v>
       </c>
@@ -3546,49 +2263,13 @@
       <c r="P31" t="n">
         <v>0</v>
       </c>
-      <c r="AB31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC31" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI31" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO31" t="n">
-        <v>0</v>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B32" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3612,11 +2293,6 @@
           <t>MARAWI CITY</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H32" t="n">
         <v>1</v>
       </c>
@@ -3638,55 +2314,19 @@
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P32" t="n">
         <v>0</v>
       </c>
-      <c r="AB32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO32" t="n">
-        <v>0</v>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B33" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3710,11 +2350,6 @@
           <t>MAIMBUNG</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>1st</t>
-        </is>
-      </c>
       <c r="H33" t="n">
         <v>1</v>
       </c>
@@ -3742,49 +2377,13 @@
       <c r="P33" t="n">
         <v>0</v>
       </c>
-      <c r="AB33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC33" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI33" t="n">
-        <v>4</v>
-      </c>
-      <c r="AJ33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO33" t="n">
-        <v>0</v>
+      <c r="AB33" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B34" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3803,11 +2402,6 @@
       <c r="F34" t="inlineStr">
         <is>
           <t>MAIMBUNG</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>1st</t>
         </is>
       </c>
       <c r="H34" t="n">
@@ -3837,49 +2431,13 @@
       <c r="P34" t="n">
         <v>0</v>
       </c>
-      <c r="AB34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI34" t="n">
-        <v>10</v>
-      </c>
-      <c r="AJ34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO34" t="n">
-        <v>0</v>
+      <c r="AB34" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B35" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3898,11 +2456,6 @@
       <c r="F35" t="inlineStr">
         <is>
           <t>PATIKUL</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>1st</t>
         </is>
       </c>
       <c r="H35" t="n">
@@ -3932,49 +2485,13 @@
       <c r="P35" t="n">
         <v>0</v>
       </c>
-      <c r="AB35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI35" t="n">
-        <v>4</v>
-      </c>
-      <c r="AJ35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO35" t="n">
-        <v>0</v>
+      <c r="AB35" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B36" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -3998,11 +2515,6 @@
           <t>LUUK</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H36" t="n">
         <v>1</v>
       </c>
@@ -4030,49 +2542,13 @@
       <c r="P36" t="n">
         <v>0</v>
       </c>
-      <c r="AB36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC36" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI36" t="n">
-        <v>12</v>
-      </c>
-      <c r="AJ36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO36" t="n">
-        <v>0</v>
+      <c r="AB36" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B37" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -4096,11 +2572,6 @@
           <t>LUUK</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H37" t="n">
         <v>1</v>
       </c>
@@ -4122,55 +2593,19 @@
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P37" t="n">
         <v>0</v>
       </c>
-      <c r="AB37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO37" t="n">
-        <v>0</v>
+      <c r="AB37" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B38" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -4194,11 +2629,6 @@
           <t>LUUK</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>2nd</t>
-        </is>
-      </c>
       <c r="H38" t="n">
         <v>1</v>
       </c>
@@ -4220,55 +2650,19 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P38" t="n">
         <v>0</v>
       </c>
-      <c r="AB38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO38" t="n">
-        <v>0</v>
+      <c r="AB38" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B39" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -4292,11 +2686,6 @@
           <t>BONGAO</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
       <c r="H39" t="n">
         <v>1</v>
       </c>
@@ -4318,55 +2707,19 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P39" t="n">
         <v>0</v>
       </c>
-      <c r="AB39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO39" t="n">
-        <v>0</v>
+      <c r="AB39" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B40" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -4390,11 +2743,6 @@
           <t>BONGAO</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
       <c r="H40" t="n">
         <v>1</v>
       </c>
@@ -4416,55 +2764,19 @@
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>On Going</t>
+          <t>Ongoing</t>
         </is>
       </c>
       <c r="P40" t="n">
         <v>0</v>
       </c>
-      <c r="AB40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO40" t="n">
-        <v>0</v>
+      <c r="AB40" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B41" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -4488,11 +2800,6 @@
           <t>BONGAO</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
       <c r="H41" t="n">
         <v>1</v>
       </c>
@@ -4520,49 +2827,13 @@
       <c r="P41" t="n">
         <v>0</v>
       </c>
-      <c r="AB41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC41" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI41" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO41" t="n">
-        <v>0</v>
+      <c r="AB41" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B42" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -4586,11 +2857,6 @@
           <t>BONGAO</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
       <c r="H42" t="n">
         <v>1</v>
       </c>
@@ -4618,49 +2884,13 @@
       <c r="P42" t="n">
         <v>0</v>
       </c>
-      <c r="AB42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC42" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI42" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO42" t="n">
-        <v>0</v>
+      <c r="AB42" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B43" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -4684,11 +2914,6 @@
           <t>LANGUYAN</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
       <c r="H43" t="n">
         <v>1</v>
       </c>
@@ -4716,49 +2941,13 @@
       <c r="P43" t="n">
         <v>0</v>
       </c>
-      <c r="AB43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC43" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI43" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO43" t="n">
-        <v>0</v>
+      <c r="AB43" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B44" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -4777,11 +2966,6 @@
       <c r="F44" t="inlineStr">
         <is>
           <t>MAPUN (CAGAYAN DE TAWI-TAWI)</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Lone</t>
         </is>
       </c>
       <c r="H44" t="n">
@@ -4811,49 +2995,13 @@
       <c r="P44" t="n">
         <v>0</v>
       </c>
-      <c r="AB44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC44" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI44" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO44" t="n">
-        <v>0</v>
+      <c r="AB44" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B45" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -4877,11 +3025,6 @@
           <t>SIMUNUL</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
       <c r="H45" t="n">
         <v>1</v>
       </c>
@@ -4909,49 +3052,13 @@
       <c r="P45" t="n">
         <v>0</v>
       </c>
-      <c r="AB45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI45" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO45" t="n">
-        <v>0</v>
+      <c r="AB45" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B46" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -4975,11 +3082,6 @@
           <t>SITANGKAI</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
       <c r="H46" t="n">
         <v>1</v>
       </c>
@@ -5007,49 +3109,13 @@
       <c r="P46" t="n">
         <v>0</v>
       </c>
-      <c r="AB46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI46" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO46" t="n">
-        <v>0</v>
+      <c r="AB46" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B47" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -5073,11 +3139,6 @@
           <t>SITANGKAI</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Lone</t>
-        </is>
-      </c>
       <c r="H47" t="n">
         <v>1</v>
       </c>
@@ -5105,49 +3166,13 @@
       <c r="P47" t="n">
         <v>0</v>
       </c>
-      <c r="AB47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI47" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO47" t="n">
-        <v>0</v>
+      <c r="AB47" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>NEWCON 2024</t>
-        </is>
-      </c>
       <c r="B48" t="inlineStr">
         <is>
           <t>BARMM</t>
@@ -5166,11 +3191,6 @@
       <c r="F48" t="inlineStr">
         <is>
           <t>SOUTH UBIAN</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Lone</t>
         </is>
       </c>
       <c r="H48" t="n">
@@ -5200,46 +3220,15 @@
       <c r="P48" t="n">
         <v>0</v>
       </c>
-      <c r="AB48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI48" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO48" t="n">
-        <v>0</v>
+      <c r="AB48" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="AT2:AT48" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AC2:AC48" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>=DropdownOptions!$A$1:$A$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
temporarily removed NIR and regenerated all regions
</commit_message>
<xml_diff>
--- a/Filtered_By_Region/BARMM/BARMM_NEWCON.xlsx
+++ b/Filtered_By_Region/BARMM/BARMM_NEWCON.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC48"/>
+  <dimension ref="A1:AD48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -449,244 +449,252 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="21" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="42" customWidth="1" min="6" max="6"/>
-    <col width="30" customWidth="1" min="7" max="7"/>
-    <col width="6" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
-    <col width="27" customWidth="1" min="10" max="10"/>
-    <col width="15" customWidth="1" min="11" max="11"/>
-    <col width="9" customWidth="1" min="12" max="12"/>
-    <col width="26" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="17" customWidth="1" min="15" max="15"/>
+    <col width="23" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="42" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="6" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="27" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="9" customWidth="1" min="13" max="13"/>
+    <col width="26" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
     <col width="17" customWidth="1" min="16" max="16"/>
-    <col width="26" customWidth="1" min="17" max="17"/>
+    <col width="17" customWidth="1" min="17" max="17"/>
     <col width="26" customWidth="1" min="18" max="18"/>
-    <col width="27" customWidth="1" min="19" max="19"/>
-    <col width="12" customWidth="1" min="20" max="20"/>
-    <col width="13" customWidth="1" min="21" max="21"/>
-    <col width="31" customWidth="1" min="22" max="22"/>
-    <col width="27" customWidth="1" min="23" max="23"/>
-    <col width="13" customWidth="1" min="24" max="24"/>
-    <col width="33" customWidth="1" min="25" max="25"/>
-    <col width="31" customWidth="1" min="26" max="26"/>
-    <col width="20" customWidth="1" min="27" max="27"/>
-    <col width="15" customWidth="1" min="28" max="28"/>
-    <col width="28" customWidth="1" min="29" max="29"/>
+    <col width="26" customWidth="1" min="19" max="19"/>
+    <col width="27" customWidth="1" min="20" max="20"/>
+    <col width="12" customWidth="1" min="21" max="21"/>
+    <col width="13" customWidth="1" min="22" max="22"/>
+    <col width="31" customWidth="1" min="23" max="23"/>
+    <col width="27" customWidth="1" min="24" max="24"/>
+    <col width="13" customWidth="1" min="25" max="25"/>
+    <col width="33" customWidth="1" min="26" max="26"/>
+    <col width="31" customWidth="1" min="27" max="27"/>
+    <col width="20" customWidth="1" min="28" max="28"/>
+    <col width="15" customWidth="1" min="29" max="29"/>
+    <col width="28" customWidth="1" min="30" max="30"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Program-Year</t>
+          <t>INDEX (DO NOT MODIFY)</t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
+          <t>PROGRAM-YEAR</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
           <t>CATEGORY</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Region</t>
-        </is>
-      </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
+          <t>REGION</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
           <t>DIVISION</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>SCHOOL ID</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>SCHOOL NAME</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>MUNICIPALITY</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>LD</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>NO. OF SITES</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>PHYSICAL TARGET
 (# OF CL)</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>SCOPE OF WORK</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Batch</t>
-        </is>
-      </c>
       <c r="M1" s="2" t="inlineStr">
         <is>
-          <t>Total Project Allocation</t>
+          <t>BATCH</t>
         </is>
       </c>
       <c r="N1" s="2" t="inlineStr">
         <is>
-          <t>Total Project Cost</t>
+          <t>TOTAL PROJECT ALLOCATION</t>
         </is>
       </c>
       <c r="O1" s="2" t="inlineStr">
         <is>
+          <t>TOTAL PROJECT COST</t>
+        </is>
+      </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
           <t>CONTRACT AMOUNT</t>
         </is>
       </c>
-      <c r="P1" s="2" t="inlineStr">
+      <c r="Q1" s="2" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="Q1" s="2" t="inlineStr">
+      <c r="R1" s="2" t="inlineStr">
         <is>
           <t>PERCENTAGE OF COMPLETION</t>
         </is>
       </c>
-      <c r="R1" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Target Completion Date </t>
-        </is>
-      </c>
       <c r="S1" s="2" t="inlineStr">
         <is>
-          <t>Actual Date of Completion</t>
+          <t xml:space="preserve"> TARGET COMPLETION DATE </t>
         </is>
       </c>
       <c r="T1" s="2" t="inlineStr">
         <is>
-          <t>Project ID</t>
+          <t>ACTUAL DATE OF COMPLETION</t>
         </is>
       </c>
       <c r="U1" s="2" t="inlineStr">
         <is>
-          <t>Contract ID</t>
+          <t>PROJECT ID</t>
         </is>
       </c>
       <c r="V1" s="2" t="inlineStr">
         <is>
-          <t>Issuance of Invitation to Bid</t>
+          <t>CONTRACT ID</t>
         </is>
       </c>
       <c r="W1" s="2" t="inlineStr">
         <is>
-          <t>Pre-Submission Conference</t>
+          <t>ISSUANCE OF INVITATION TO BID</t>
         </is>
       </c>
       <c r="X1" s="2" t="inlineStr">
         <is>
-          <t>Bid Opening</t>
+          <t>PRE-SUBMISSION CONFERENCE</t>
         </is>
       </c>
       <c r="Y1" s="2" t="inlineStr">
         <is>
-          <t>Issuance of Resolution to Award</t>
+          <t>BID OPENING</t>
         </is>
       </c>
       <c r="Z1" s="2" t="inlineStr">
         <is>
-          <t>Issuance of Notice to Proceed</t>
+          <t>ISSUANCE OF RESOLUTION TO AWARD</t>
         </is>
       </c>
       <c r="AA1" s="2" t="inlineStr">
         <is>
-          <t>Name of Contractor</t>
+          <t>ISSUANCE OF NOTICE TO PROCEED</t>
         </is>
       </c>
       <c r="AB1" s="2" t="inlineStr">
         <is>
-          <t>Other Remarks</t>
-        </is>
-      </c>
-      <c r="AC1" s="3" t="inlineStr">
+          <t>NAME OF CONTRACTOR</t>
+        </is>
+      </c>
+      <c r="AC1" s="2" t="inlineStr">
+        <is>
+          <t>OTHER REMARKS</t>
+        </is>
+      </c>
+      <c r="AD1" s="3" t="inlineStr">
         <is>
           <t>Status as of July 11, 2025</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="inlineStr"/>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A2" s="4" t="n">
+        <v>43058</v>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr"/>
       <c r="D2" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
           <t>Isabela City</t>
         </is>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="F2" s="4" t="n">
         <v>303894</v>
       </c>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>Basilan NHS</t>
         </is>
       </c>
-      <c r="G2" s="4" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>CITY OF ISABELA (Capital)</t>
         </is>
       </c>
-      <c r="H2" s="4" t="inlineStr"/>
-      <c r="I2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="4" t="inlineStr"/>
-      <c r="K2" s="4" t="inlineStr">
+      <c r="I2" s="4" t="inlineStr"/>
+      <c r="J2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4" t="inlineStr"/>
+      <c r="L2" s="4" t="inlineStr">
         <is>
           <t>1-UNIT 4STY</t>
         </is>
       </c>
-      <c r="L2" s="4" t="inlineStr">
+      <c r="M2" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M2" s="4" t="n">
+      <c r="N2" s="4" t="n">
         <v>40000000</v>
       </c>
-      <c r="N2" s="4" t="inlineStr"/>
       <c r="O2" s="4" t="inlineStr"/>
-      <c r="P2" s="4" t="inlineStr">
+      <c r="P2" s="4" t="inlineStr"/>
+      <c r="Q2" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="4" t="inlineStr"/>
+      <c r="R2" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S2" s="4" t="inlineStr"/>
       <c r="T2" s="4" t="inlineStr"/>
       <c r="U2" s="4" t="inlineStr"/>
@@ -697,69 +705,72 @@
       <c r="Z2" s="4" t="inlineStr"/>
       <c r="AA2" s="4" t="inlineStr"/>
       <c r="AB2" s="4" t="inlineStr"/>
-      <c r="AC2" s="5" t="n"/>
+      <c r="AC2" s="4" t="inlineStr"/>
+      <c r="AD2" s="5" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr"/>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A3" s="4" t="n">
+        <v>43059</v>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr"/>
       <c r="D3" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
           <t>Lamitan City</t>
         </is>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="F3" s="4" t="n">
         <v>304940</v>
       </c>
-      <c r="F3" s="4" t="inlineStr">
+      <c r="G3" s="4" t="inlineStr">
         <is>
           <t>Lo-ok National High School</t>
         </is>
       </c>
-      <c r="G3" s="4" t="inlineStr">
+      <c r="H3" s="4" t="inlineStr">
         <is>
           <t>CITY OF LAMITAN</t>
         </is>
       </c>
-      <c r="H3" s="4" t="inlineStr"/>
-      <c r="I3" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I3" s="4" t="inlineStr"/>
       <c r="J3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="K3" s="4" t="inlineStr">
+      <c r="L3" s="4" t="inlineStr">
         <is>
           <t>4STY16CL</t>
         </is>
       </c>
-      <c r="L3" s="4" t="inlineStr">
+      <c r="M3" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M3" s="4" t="n">
+      <c r="N3" s="4" t="n">
         <v>40000000</v>
       </c>
-      <c r="N3" s="4" t="inlineStr"/>
       <c r="O3" s="4" t="inlineStr"/>
-      <c r="P3" s="4" t="inlineStr">
+      <c r="P3" s="4" t="inlineStr"/>
+      <c r="Q3" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="4" t="inlineStr"/>
+      <c r="R3" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S3" s="4" t="inlineStr"/>
       <c r="T3" s="4" t="inlineStr"/>
       <c r="U3" s="4" t="inlineStr"/>
@@ -770,65 +781,68 @@
       <c r="Z3" s="4" t="inlineStr"/>
       <c r="AA3" s="4" t="inlineStr"/>
       <c r="AB3" s="4" t="inlineStr"/>
-      <c r="AC3" s="5" t="n"/>
+      <c r="AC3" s="4" t="inlineStr"/>
+      <c r="AD3" s="5" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr"/>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A4" s="4" t="n">
+        <v>43060</v>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr"/>
       <c r="D4" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - I</t>
         </is>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="F4" s="4" t="n">
         <v>133540</v>
       </c>
-      <c r="F4" s="4" t="inlineStr"/>
-      <c r="G4" s="4" t="inlineStr">
+      <c r="G4" s="4" t="inlineStr"/>
+      <c r="H4" s="4" t="inlineStr">
         <is>
           <t>BUMBARAN</t>
         </is>
       </c>
-      <c r="H4" s="4" t="inlineStr"/>
-      <c r="I4" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I4" s="4" t="inlineStr"/>
       <c r="J4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K4" s="4" t="inlineStr">
+      <c r="L4" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L4" s="4" t="inlineStr">
+      <c r="M4" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M4" s="4" t="n">
+      <c r="N4" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N4" s="4" t="inlineStr"/>
       <c r="O4" s="4" t="inlineStr"/>
-      <c r="P4" s="4" t="inlineStr">
+      <c r="P4" s="4" t="inlineStr"/>
+      <c r="Q4" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="4" t="inlineStr"/>
+      <c r="R4" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S4" s="4" t="inlineStr"/>
       <c r="T4" s="4" t="inlineStr"/>
       <c r="U4" s="4" t="inlineStr"/>
@@ -839,69 +853,72 @@
       <c r="Z4" s="4" t="inlineStr"/>
       <c r="AA4" s="4" t="inlineStr"/>
       <c r="AB4" s="4" t="inlineStr"/>
-      <c r="AC4" s="5" t="n"/>
+      <c r="AC4" s="4" t="inlineStr"/>
+      <c r="AD4" s="5" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr"/>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A5" s="4" t="n">
+        <v>43061</v>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr"/>
       <c r="D5" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - I</t>
         </is>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="F5" s="4" t="n">
         <v>133541</v>
       </c>
-      <c r="F5" s="4" t="inlineStr">
+      <c r="G5" s="4" t="inlineStr">
         <is>
           <t>Natangcopan PS</t>
         </is>
       </c>
-      <c r="G5" s="4" t="inlineStr">
+      <c r="H5" s="4" t="inlineStr">
         <is>
           <t>BUMBARAN</t>
         </is>
       </c>
-      <c r="H5" s="4" t="inlineStr"/>
-      <c r="I5" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I5" s="4" t="inlineStr"/>
       <c r="J5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K5" s="4" t="inlineStr">
+      <c r="L5" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L5" s="4" t="inlineStr">
+      <c r="M5" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M5" s="4" t="n">
+      <c r="N5" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N5" s="4" t="inlineStr"/>
       <c r="O5" s="4" t="inlineStr"/>
-      <c r="P5" s="4" t="inlineStr">
+      <c r="P5" s="4" t="inlineStr"/>
+      <c r="Q5" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="4" t="inlineStr"/>
+      <c r="R5" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S5" s="4" t="inlineStr"/>
       <c r="T5" s="4" t="inlineStr"/>
       <c r="U5" s="4" t="inlineStr"/>
@@ -912,69 +929,72 @@
       <c r="Z5" s="4" t="inlineStr"/>
       <c r="AA5" s="4" t="inlineStr"/>
       <c r="AB5" s="4" t="inlineStr"/>
-      <c r="AC5" s="5" t="n"/>
+      <c r="AC5" s="4" t="inlineStr"/>
+      <c r="AD5" s="5" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr"/>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A6" s="4" t="n">
+        <v>43062</v>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr"/>
       <c r="D6" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - I</t>
         </is>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="F6" s="4" t="n">
         <v>133276</v>
       </c>
-      <c r="F6" s="4" t="inlineStr">
+      <c r="G6" s="4" t="inlineStr">
         <is>
           <t>Sultan Alauya Alonto CES</t>
         </is>
       </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="H6" s="4" t="inlineStr">
         <is>
           <t>DITSAAN-RAMAIN</t>
         </is>
       </c>
-      <c r="H6" s="4" t="inlineStr"/>
-      <c r="I6" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I6" s="4" t="inlineStr"/>
       <c r="J6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="K6" s="4" t="inlineStr">
+      <c r="L6" s="4" t="inlineStr">
         <is>
           <t>2STY8CL</t>
         </is>
       </c>
-      <c r="L6" s="4" t="inlineStr">
+      <c r="M6" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="N6" s="4" t="n">
         <v>30000000</v>
       </c>
-      <c r="N6" s="4" t="inlineStr"/>
       <c r="O6" s="4" t="inlineStr"/>
-      <c r="P6" s="4" t="inlineStr">
+      <c r="P6" s="4" t="inlineStr"/>
+      <c r="Q6" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="4" t="inlineStr"/>
+      <c r="R6" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S6" s="4" t="inlineStr"/>
       <c r="T6" s="4" t="inlineStr"/>
       <c r="U6" s="4" t="inlineStr"/>
@@ -985,69 +1005,72 @@
       <c r="Z6" s="4" t="inlineStr"/>
       <c r="AA6" s="4" t="inlineStr"/>
       <c r="AB6" s="4" t="inlineStr"/>
-      <c r="AC6" s="5" t="n"/>
+      <c r="AC6" s="4" t="inlineStr"/>
+      <c r="AD6" s="5" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr"/>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A7" s="4" t="n">
+        <v>43063</v>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr"/>
       <c r="D7" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - I</t>
         </is>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="F7" s="4" t="n">
         <v>133348</v>
       </c>
-      <c r="F7" s="4" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr">
         <is>
           <t>Loway Inudaran ES</t>
         </is>
       </c>
-      <c r="G7" s="4" t="inlineStr">
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>MARANTAO</t>
         </is>
       </c>
-      <c r="H7" s="4" t="inlineStr"/>
-      <c r="I7" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I7" s="4" t="inlineStr"/>
       <c r="J7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="K7" s="4" t="inlineStr">
+      <c r="L7" s="4" t="inlineStr">
         <is>
           <t>2STY8CL</t>
         </is>
       </c>
-      <c r="L7" s="4" t="inlineStr">
+      <c r="M7" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M7" s="4" t="n">
+      <c r="N7" s="4" t="n">
         <v>30000000</v>
       </c>
-      <c r="N7" s="4" t="inlineStr"/>
       <c r="O7" s="4" t="inlineStr"/>
-      <c r="P7" s="4" t="inlineStr">
+      <c r="P7" s="4" t="inlineStr"/>
+      <c r="Q7" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="4" t="inlineStr"/>
+      <c r="R7" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S7" s="4" t="inlineStr"/>
       <c r="T7" s="4" t="inlineStr"/>
       <c r="U7" s="4" t="inlineStr"/>
@@ -1058,69 +1081,72 @@
       <c r="Z7" s="4" t="inlineStr"/>
       <c r="AA7" s="4" t="inlineStr"/>
       <c r="AB7" s="4" t="inlineStr"/>
-      <c r="AC7" s="5" t="n"/>
+      <c r="AC7" s="4" t="inlineStr"/>
+      <c r="AD7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B8" s="4" t="inlineStr"/>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A8" s="4" t="n">
+        <v>43064</v>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr"/>
       <c r="D8" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - I</t>
         </is>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="F8" s="4" t="n">
         <v>133425</v>
       </c>
-      <c r="F8" s="4" t="inlineStr">
+      <c r="G8" s="4" t="inlineStr">
         <is>
           <t>Ragayan CES</t>
         </is>
       </c>
-      <c r="G8" s="4" t="inlineStr">
+      <c r="H8" s="4" t="inlineStr">
         <is>
           <t>POONA BAYABAO (GATA)</t>
         </is>
       </c>
-      <c r="H8" s="4" t="inlineStr"/>
-      <c r="I8" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I8" s="4" t="inlineStr"/>
       <c r="J8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K8" s="4" t="inlineStr">
+      <c r="L8" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L8" s="4" t="inlineStr">
+      <c r="M8" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M8" s="4" t="n">
+      <c r="N8" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N8" s="4" t="inlineStr"/>
       <c r="O8" s="4" t="inlineStr"/>
-      <c r="P8" s="4" t="inlineStr">
+      <c r="P8" s="4" t="inlineStr"/>
+      <c r="Q8" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="4" t="inlineStr"/>
+      <c r="R8" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S8" s="4" t="inlineStr"/>
       <c r="T8" s="4" t="inlineStr"/>
       <c r="U8" s="4" t="inlineStr"/>
@@ -1131,69 +1157,72 @@
       <c r="Z8" s="4" t="inlineStr"/>
       <c r="AA8" s="4" t="inlineStr"/>
       <c r="AB8" s="4" t="inlineStr"/>
-      <c r="AC8" s="5" t="n"/>
+      <c r="AC8" s="4" t="inlineStr"/>
+      <c r="AD8" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr"/>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A9" s="4" t="n">
+        <v>43065</v>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr"/>
       <c r="D9" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - I</t>
         </is>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="F9" s="4" t="n">
         <v>304972</v>
       </c>
-      <c r="F9" s="4" t="inlineStr">
+      <c r="G9" s="4" t="inlineStr">
         <is>
           <t>Pagalongan NHS</t>
         </is>
       </c>
-      <c r="G9" s="4" t="inlineStr">
+      <c r="H9" s="4" t="inlineStr">
         <is>
           <t>WAO</t>
         </is>
       </c>
-      <c r="H9" s="4" t="inlineStr"/>
-      <c r="I9" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I9" s="4" t="inlineStr"/>
       <c r="J9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="K9" s="4" t="inlineStr">
+      <c r="L9" s="4" t="inlineStr">
         <is>
           <t>3STY12CL</t>
         </is>
       </c>
-      <c r="L9" s="4" t="inlineStr">
+      <c r="M9" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M9" s="4" t="n">
+      <c r="N9" s="4" t="n">
         <v>42000000</v>
       </c>
-      <c r="N9" s="4" t="inlineStr"/>
       <c r="O9" s="4" t="inlineStr"/>
-      <c r="P9" s="4" t="inlineStr">
+      <c r="P9" s="4" t="inlineStr"/>
+      <c r="Q9" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" s="4" t="inlineStr"/>
+      <c r="R9" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S9" s="4" t="inlineStr"/>
       <c r="T9" s="4" t="inlineStr"/>
       <c r="U9" s="4" t="inlineStr"/>
@@ -1204,69 +1233,72 @@
       <c r="Z9" s="4" t="inlineStr"/>
       <c r="AA9" s="4" t="inlineStr"/>
       <c r="AB9" s="4" t="inlineStr"/>
-      <c r="AC9" s="5" t="n"/>
+      <c r="AC9" s="4" t="inlineStr"/>
+      <c r="AD9" s="5" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr"/>
-      <c r="C10" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A10" s="4" t="n">
+        <v>43066</v>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr"/>
       <c r="D10" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - I</t>
         </is>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="F10" s="4" t="n">
         <v>133537</v>
       </c>
-      <c r="F10" s="4" t="inlineStr">
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t>South Park Area ES</t>
         </is>
       </c>
-      <c r="G10" s="4" t="inlineStr">
+      <c r="H10" s="4" t="inlineStr">
         <is>
           <t>WAO</t>
         </is>
       </c>
-      <c r="H10" s="4" t="inlineStr"/>
-      <c r="I10" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I10" s="4" t="inlineStr"/>
       <c r="J10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K10" s="4" t="inlineStr">
+      <c r="L10" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L10" s="4" t="inlineStr">
+      <c r="M10" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M10" s="4" t="n">
+      <c r="N10" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N10" s="4" t="inlineStr"/>
       <c r="O10" s="4" t="inlineStr"/>
-      <c r="P10" s="4" t="inlineStr">
+      <c r="P10" s="4" t="inlineStr"/>
+      <c r="Q10" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" s="4" t="inlineStr"/>
+      <c r="R10" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S10" s="4" t="inlineStr"/>
       <c r="T10" s="4" t="inlineStr"/>
       <c r="U10" s="4" t="inlineStr"/>
@@ -1277,69 +1309,72 @@
       <c r="Z10" s="4" t="inlineStr"/>
       <c r="AA10" s="4" t="inlineStr"/>
       <c r="AB10" s="4" t="inlineStr"/>
-      <c r="AC10" s="5" t="n"/>
+      <c r="AC10" s="4" t="inlineStr"/>
+      <c r="AD10" s="5" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B11" s="4" t="inlineStr"/>
-      <c r="C11" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A11" s="4" t="n">
+        <v>43067</v>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr"/>
       <c r="D11" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - II</t>
         </is>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="F11" s="4" t="n">
         <v>324712</v>
       </c>
-      <c r="F11" s="4" t="inlineStr">
+      <c r="G11" s="4" t="inlineStr">
         <is>
           <t>Datu Raquib Zainodin National Highschool</t>
         </is>
       </c>
-      <c r="G11" s="4" t="inlineStr">
+      <c r="H11" s="4" t="inlineStr">
         <is>
           <t>MADALUM</t>
         </is>
       </c>
-      <c r="H11" s="4" t="inlineStr"/>
-      <c r="I11" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I11" s="4" t="inlineStr"/>
       <c r="J11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K11" s="4" t="inlineStr">
+      <c r="L11" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L11" s="4" t="inlineStr">
+      <c r="M11" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M11" s="4" t="n">
+      <c r="N11" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N11" s="4" t="inlineStr"/>
       <c r="O11" s="4" t="inlineStr"/>
-      <c r="P11" s="4" t="inlineStr">
+      <c r="P11" s="4" t="inlineStr"/>
+      <c r="Q11" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" s="4" t="inlineStr"/>
+      <c r="R11" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S11" s="4" t="inlineStr"/>
       <c r="T11" s="4" t="inlineStr"/>
       <c r="U11" s="4" t="inlineStr"/>
@@ -1350,69 +1385,72 @@
       <c r="Z11" s="4" t="inlineStr"/>
       <c r="AA11" s="4" t="inlineStr"/>
       <c r="AB11" s="4" t="inlineStr"/>
-      <c r="AC11" s="5" t="n"/>
+      <c r="AC11" s="4" t="inlineStr"/>
+      <c r="AD11" s="5" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr"/>
-      <c r="C12" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A12" s="4" t="n">
+        <v>43068</v>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="inlineStr"/>
       <c r="D12" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - II</t>
         </is>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="F12" s="4" t="n">
         <v>133723</v>
       </c>
-      <c r="F12" s="4" t="inlineStr">
+      <c r="G12" s="4" t="inlineStr">
         <is>
           <t>Liangan Primary School</t>
         </is>
       </c>
-      <c r="G12" s="4" t="inlineStr">
+      <c r="H12" s="4" t="inlineStr">
         <is>
           <t>MADAMBA</t>
         </is>
       </c>
-      <c r="H12" s="4" t="inlineStr"/>
-      <c r="I12" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I12" s="4" t="inlineStr"/>
       <c r="J12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K12" s="4" t="inlineStr">
+      <c r="L12" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L12" s="4" t="inlineStr">
+      <c r="M12" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M12" s="4" t="n">
+      <c r="N12" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N12" s="4" t="inlineStr"/>
       <c r="O12" s="4" t="inlineStr"/>
-      <c r="P12" s="4" t="inlineStr">
+      <c r="P12" s="4" t="inlineStr"/>
+      <c r="Q12" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="4" t="inlineStr"/>
+      <c r="R12" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S12" s="4" t="inlineStr"/>
       <c r="T12" s="4" t="inlineStr"/>
       <c r="U12" s="4" t="inlineStr"/>
@@ -1423,67 +1461,70 @@
       <c r="Z12" s="4" t="inlineStr"/>
       <c r="AA12" s="4" t="inlineStr"/>
       <c r="AB12" s="4" t="inlineStr"/>
-      <c r="AC12" s="5" t="n"/>
+      <c r="AC12" s="4" t="inlineStr"/>
+      <c r="AD12" s="5" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B13" s="4" t="inlineStr"/>
-      <c r="C13" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A13" s="4" t="n">
+        <v>43069</v>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C13" s="4" t="inlineStr"/>
       <c r="D13" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - II</t>
         </is>
       </c>
-      <c r="E13" s="4" t="inlineStr"/>
-      <c r="F13" s="4" t="inlineStr">
+      <c r="F13" s="4" t="inlineStr"/>
+      <c r="G13" s="4" t="inlineStr">
         <is>
           <t>Pagayonan National High School</t>
         </is>
       </c>
-      <c r="G13" s="4" t="inlineStr">
+      <c r="H13" s="4" t="inlineStr">
         <is>
           <t>MADAMBA</t>
         </is>
       </c>
-      <c r="H13" s="4" t="inlineStr"/>
-      <c r="I13" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I13" s="4" t="inlineStr"/>
       <c r="J13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K13" s="4" t="inlineStr">
+      <c r="L13" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L13" s="4" t="inlineStr">
+      <c r="M13" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M13" s="4" t="n">
+      <c r="N13" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N13" s="4" t="inlineStr"/>
       <c r="O13" s="4" t="inlineStr"/>
-      <c r="P13" s="4" t="inlineStr">
+      <c r="P13" s="4" t="inlineStr"/>
+      <c r="Q13" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="4" t="inlineStr"/>
+      <c r="R13" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S13" s="4" t="inlineStr"/>
       <c r="T13" s="4" t="inlineStr"/>
       <c r="U13" s="4" t="inlineStr"/>
@@ -1494,69 +1535,72 @@
       <c r="Z13" s="4" t="inlineStr"/>
       <c r="AA13" s="4" t="inlineStr"/>
       <c r="AB13" s="4" t="inlineStr"/>
-      <c r="AC13" s="5" t="n"/>
+      <c r="AC13" s="4" t="inlineStr"/>
+      <c r="AD13" s="5" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B14" s="4" t="inlineStr"/>
-      <c r="C14" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A14" s="4" t="n">
+        <v>43070</v>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="inlineStr"/>
       <c r="D14" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E14" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - II</t>
         </is>
       </c>
-      <c r="E14" s="4" t="n">
+      <c r="F14" s="4" t="n">
         <v>133753</v>
       </c>
-      <c r="F14" s="4" t="inlineStr">
+      <c r="G14" s="4" t="inlineStr">
         <is>
           <t>Calimodan Vil. ES</t>
         </is>
       </c>
-      <c r="G14" s="4" t="inlineStr">
+      <c r="H14" s="4" t="inlineStr">
         <is>
           <t>MALABANG</t>
         </is>
       </c>
-      <c r="H14" s="4" t="inlineStr"/>
-      <c r="I14" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I14" s="4" t="inlineStr"/>
       <c r="J14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K14" s="4" t="inlineStr">
+      <c r="L14" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L14" s="4" t="inlineStr">
+      <c r="M14" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M14" s="4" t="n">
+      <c r="N14" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N14" s="4" t="inlineStr"/>
       <c r="O14" s="4" t="inlineStr"/>
-      <c r="P14" s="4" t="inlineStr">
+      <c r="P14" s="4" t="inlineStr"/>
+      <c r="Q14" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q14" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" s="4" t="inlineStr"/>
+      <c r="R14" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S14" s="4" t="inlineStr"/>
       <c r="T14" s="4" t="inlineStr"/>
       <c r="U14" s="4" t="inlineStr"/>
@@ -1567,69 +1611,72 @@
       <c r="Z14" s="4" t="inlineStr"/>
       <c r="AA14" s="4" t="inlineStr"/>
       <c r="AB14" s="4" t="inlineStr"/>
-      <c r="AC14" s="5" t="n"/>
+      <c r="AC14" s="4" t="inlineStr"/>
+      <c r="AD14" s="5" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B15" s="4" t="inlineStr"/>
-      <c r="C15" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A15" s="4" t="n">
+        <v>43071</v>
+      </c>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C15" s="4" t="inlineStr"/>
       <c r="D15" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - II</t>
         </is>
       </c>
-      <c r="E15" s="4" t="n">
+      <c r="F15" s="4" t="n">
         <v>133821</v>
       </c>
-      <c r="F15" s="4" t="inlineStr">
+      <c r="G15" s="4" t="inlineStr">
         <is>
           <t>Baraas Central School</t>
         </is>
       </c>
-      <c r="G15" s="4" t="inlineStr">
+      <c r="H15" s="4" t="inlineStr">
         <is>
           <t>SULTAN GUMANDER (PICONG)</t>
         </is>
       </c>
-      <c r="H15" s="4" t="inlineStr"/>
-      <c r="I15" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I15" s="4" t="inlineStr"/>
       <c r="J15" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K15" s="4" t="inlineStr">
+      <c r="L15" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L15" s="4" t="inlineStr">
+      <c r="M15" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M15" s="4" t="n">
+      <c r="N15" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N15" s="4" t="inlineStr"/>
       <c r="O15" s="4" t="inlineStr"/>
-      <c r="P15" s="4" t="inlineStr">
+      <c r="P15" s="4" t="inlineStr"/>
+      <c r="Q15" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q15" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R15" s="4" t="inlineStr"/>
+      <c r="R15" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S15" s="4" t="inlineStr"/>
       <c r="T15" s="4" t="inlineStr"/>
       <c r="U15" s="4" t="inlineStr"/>
@@ -1640,69 +1687,72 @@
       <c r="Z15" s="4" t="inlineStr"/>
       <c r="AA15" s="4" t="inlineStr"/>
       <c r="AB15" s="4" t="inlineStr"/>
-      <c r="AC15" s="5" t="n"/>
+      <c r="AC15" s="4" t="inlineStr"/>
+      <c r="AD15" s="5" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B16" s="4" t="inlineStr"/>
-      <c r="C16" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A16" s="4" t="n">
+        <v>43072</v>
+      </c>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="inlineStr"/>
       <c r="D16" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="inlineStr">
+        <is>
           <t>Lanao del Sur - II</t>
         </is>
       </c>
-      <c r="E16" s="4" t="n">
+      <c r="F16" s="4" t="n">
         <v>318233</v>
       </c>
-      <c r="F16" s="4" t="inlineStr">
+      <c r="G16" s="4" t="inlineStr">
         <is>
           <t>Balindong Pacalna National High School</t>
         </is>
       </c>
-      <c r="G16" s="4" t="inlineStr">
+      <c r="H16" s="4" t="inlineStr">
         <is>
           <t>TUGAYA</t>
         </is>
       </c>
-      <c r="H16" s="4" t="inlineStr"/>
-      <c r="I16" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I16" s="4" t="inlineStr"/>
       <c r="J16" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K16" s="4" t="inlineStr">
+      <c r="L16" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L16" s="4" t="inlineStr">
+      <c r="M16" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M16" s="4" t="n">
+      <c r="N16" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N16" s="4" t="inlineStr"/>
       <c r="O16" s="4" t="inlineStr"/>
-      <c r="P16" s="4" t="inlineStr">
+      <c r="P16" s="4" t="inlineStr"/>
+      <c r="Q16" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q16" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" s="4" t="inlineStr"/>
+      <c r="R16" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S16" s="4" t="inlineStr"/>
       <c r="T16" s="4" t="inlineStr"/>
       <c r="U16" s="4" t="inlineStr"/>
@@ -1713,69 +1763,72 @@
       <c r="Z16" s="4" t="inlineStr"/>
       <c r="AA16" s="4" t="inlineStr"/>
       <c r="AB16" s="4" t="inlineStr"/>
-      <c r="AC16" s="5" t="n"/>
+      <c r="AC16" s="4" t="inlineStr"/>
+      <c r="AD16" s="5" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B17" s="4" t="inlineStr"/>
-      <c r="C17" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A17" s="4" t="n">
+        <v>43073</v>
+      </c>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C17" s="4" t="inlineStr"/>
       <c r="D17" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao del Sur</t>
         </is>
       </c>
-      <c r="E17" s="4" t="n">
+      <c r="F17" s="4" t="n">
         <v>305012</v>
       </c>
-      <c r="F17" s="4" t="inlineStr">
+      <c r="G17" s="4" t="inlineStr">
         <is>
           <t>Kauran NHS</t>
         </is>
       </c>
-      <c r="G17" s="4" t="inlineStr">
+      <c r="H17" s="4" t="inlineStr">
         <is>
           <t>AMPATUAN</t>
         </is>
       </c>
-      <c r="H17" s="4" t="inlineStr"/>
-      <c r="I17" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I17" s="4" t="inlineStr"/>
       <c r="J17" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="K17" s="4" t="inlineStr">
+      <c r="L17" s="4" t="inlineStr">
         <is>
           <t>1STY4CL</t>
         </is>
       </c>
-      <c r="L17" s="4" t="inlineStr">
+      <c r="M17" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M17" s="4" t="n">
+      <c r="N17" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N17" s="4" t="inlineStr"/>
       <c r="O17" s="4" t="inlineStr"/>
-      <c r="P17" s="4" t="inlineStr">
+      <c r="P17" s="4" t="inlineStr"/>
+      <c r="Q17" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q17" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" s="4" t="inlineStr"/>
+      <c r="R17" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S17" s="4" t="inlineStr"/>
       <c r="T17" s="4" t="inlineStr"/>
       <c r="U17" s="4" t="inlineStr"/>
@@ -1786,69 +1839,72 @@
       <c r="Z17" s="4" t="inlineStr"/>
       <c r="AA17" s="4" t="inlineStr"/>
       <c r="AB17" s="4" t="inlineStr"/>
-      <c r="AC17" s="5" t="n"/>
+      <c r="AC17" s="4" t="inlineStr"/>
+      <c r="AD17" s="5" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B18" s="4" t="inlineStr"/>
-      <c r="C18" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A18" s="4" t="n">
+        <v>43074</v>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C18" s="4" t="inlineStr"/>
       <c r="D18" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao del Sur</t>
         </is>
       </c>
-      <c r="E18" s="4" t="n">
+      <c r="F18" s="4" t="n">
         <v>133933</v>
       </c>
-      <c r="F18" s="4" t="inlineStr">
+      <c r="G18" s="4" t="inlineStr">
         <is>
           <t>Bai Bagongan Paglas ES</t>
         </is>
       </c>
-      <c r="G18" s="4" t="inlineStr">
+      <c r="H18" s="4" t="inlineStr">
         <is>
           <t>BULUAN</t>
         </is>
       </c>
-      <c r="H18" s="4" t="inlineStr"/>
-      <c r="I18" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I18" s="4" t="inlineStr"/>
       <c r="J18" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="K18" s="4" t="inlineStr">
+      <c r="L18" s="4" t="inlineStr">
         <is>
           <t>1STY4CL</t>
         </is>
       </c>
-      <c r="L18" s="4" t="inlineStr">
+      <c r="M18" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M18" s="4" t="n">
+      <c r="N18" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N18" s="4" t="inlineStr"/>
       <c r="O18" s="4" t="inlineStr"/>
-      <c r="P18" s="4" t="inlineStr">
+      <c r="P18" s="4" t="inlineStr"/>
+      <c r="Q18" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" s="4" t="inlineStr"/>
+      <c r="R18" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S18" s="4" t="inlineStr"/>
       <c r="T18" s="4" t="inlineStr"/>
       <c r="U18" s="4" t="inlineStr"/>
@@ -1859,69 +1915,72 @@
       <c r="Z18" s="4" t="inlineStr"/>
       <c r="AA18" s="4" t="inlineStr"/>
       <c r="AB18" s="4" t="inlineStr"/>
-      <c r="AC18" s="5" t="n"/>
+      <c r="AC18" s="4" t="inlineStr"/>
+      <c r="AD18" s="5" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B19" s="4" t="inlineStr"/>
-      <c r="C19" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A19" s="4" t="n">
+        <v>43075</v>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C19" s="4" t="inlineStr"/>
       <c r="D19" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao del Sur</t>
         </is>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="F19" s="4" t="n">
         <v>305028</v>
       </c>
-      <c r="F19" s="4" t="inlineStr">
+      <c r="G19" s="4" t="inlineStr">
         <is>
           <t>Tunggol NHS</t>
         </is>
       </c>
-      <c r="G19" s="4" t="inlineStr">
+      <c r="H19" s="4" t="inlineStr">
         <is>
           <t>DATU MONTAWAL (PAGAGAWAN)</t>
         </is>
       </c>
-      <c r="H19" s="4" t="inlineStr"/>
-      <c r="I19" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I19" s="4" t="inlineStr"/>
       <c r="J19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="K19" s="4" t="inlineStr">
+      <c r="L19" s="4" t="inlineStr">
         <is>
           <t>1STY4CL</t>
         </is>
       </c>
-      <c r="L19" s="4" t="inlineStr">
+      <c r="M19" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M19" s="4" t="n">
+      <c r="N19" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N19" s="4" t="inlineStr"/>
       <c r="O19" s="4" t="inlineStr"/>
-      <c r="P19" s="4" t="inlineStr">
+      <c r="P19" s="4" t="inlineStr"/>
+      <c r="Q19" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" s="4" t="inlineStr"/>
+      <c r="R19" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S19" s="4" t="inlineStr"/>
       <c r="T19" s="4" t="inlineStr"/>
       <c r="U19" s="4" t="inlineStr"/>
@@ -1932,69 +1991,72 @@
       <c r="Z19" s="4" t="inlineStr"/>
       <c r="AA19" s="4" t="inlineStr"/>
       <c r="AB19" s="4" t="inlineStr"/>
-      <c r="AC19" s="5" t="n"/>
+      <c r="AC19" s="4" t="inlineStr"/>
+      <c r="AD19" s="5" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B20" s="4" t="inlineStr"/>
-      <c r="C20" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A20" s="4" t="n">
+        <v>43076</v>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="inlineStr"/>
       <c r="D20" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao del Sur</t>
         </is>
       </c>
-      <c r="E20" s="4" t="n">
+      <c r="F20" s="4" t="n">
         <v>136971</v>
       </c>
-      <c r="F20" s="4" t="inlineStr">
+      <c r="G20" s="4" t="inlineStr">
         <is>
           <t>Datu Bandala Mamasabulod ES</t>
         </is>
       </c>
-      <c r="G20" s="4" t="inlineStr">
+      <c r="H20" s="4" t="inlineStr">
         <is>
           <t>PAGALUNGAN</t>
         </is>
       </c>
-      <c r="H20" s="4" t="inlineStr"/>
-      <c r="I20" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I20" s="4" t="inlineStr"/>
       <c r="J20" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="K20" s="4" t="inlineStr">
+      <c r="L20" s="4" t="inlineStr">
         <is>
           <t>1STY4CL</t>
         </is>
       </c>
-      <c r="L20" s="4" t="inlineStr">
+      <c r="M20" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M20" s="4" t="n">
+      <c r="N20" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N20" s="4" t="inlineStr"/>
       <c r="O20" s="4" t="inlineStr"/>
-      <c r="P20" s="4" t="inlineStr">
+      <c r="P20" s="4" t="inlineStr"/>
+      <c r="Q20" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R20" s="4" t="inlineStr"/>
+      <c r="R20" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S20" s="4" t="inlineStr"/>
       <c r="T20" s="4" t="inlineStr"/>
       <c r="U20" s="4" t="inlineStr"/>
@@ -2005,69 +2067,72 @@
       <c r="Z20" s="4" t="inlineStr"/>
       <c r="AA20" s="4" t="inlineStr"/>
       <c r="AB20" s="4" t="inlineStr"/>
-      <c r="AC20" s="5" t="n"/>
+      <c r="AC20" s="4" t="inlineStr"/>
+      <c r="AD20" s="5" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B21" s="4" t="inlineStr"/>
-      <c r="C21" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A21" s="4" t="n">
+        <v>43077</v>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="inlineStr"/>
       <c r="D21" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao del Sur</t>
         </is>
       </c>
-      <c r="E21" s="4" t="n">
+      <c r="F21" s="4" t="n">
         <v>305022</v>
       </c>
-      <c r="F21" s="4" t="inlineStr">
+      <c r="G21" s="4" t="inlineStr">
         <is>
           <t>South Upi NHS</t>
         </is>
       </c>
-      <c r="G21" s="4" t="inlineStr">
+      <c r="H21" s="4" t="inlineStr">
         <is>
           <t>SOUTH UPI</t>
         </is>
       </c>
-      <c r="H21" s="4" t="inlineStr"/>
-      <c r="I21" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I21" s="4" t="inlineStr"/>
       <c r="J21" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="K21" s="4" t="inlineStr">
+      <c r="L21" s="4" t="inlineStr">
         <is>
           <t>1STY4CL</t>
         </is>
       </c>
-      <c r="L21" s="4" t="inlineStr">
+      <c r="M21" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M21" s="4" t="n">
+      <c r="N21" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N21" s="4" t="inlineStr"/>
       <c r="O21" s="4" t="inlineStr"/>
-      <c r="P21" s="4" t="inlineStr">
+      <c r="P21" s="4" t="inlineStr"/>
+      <c r="Q21" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q21" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R21" s="4" t="inlineStr"/>
+      <c r="R21" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S21" s="4" t="inlineStr"/>
       <c r="T21" s="4" t="inlineStr"/>
       <c r="U21" s="4" t="inlineStr"/>
@@ -2078,69 +2143,72 @@
       <c r="Z21" s="4" t="inlineStr"/>
       <c r="AA21" s="4" t="inlineStr"/>
       <c r="AB21" s="4" t="inlineStr"/>
-      <c r="AC21" s="5" t="n"/>
+      <c r="AC21" s="4" t="inlineStr"/>
+      <c r="AD21" s="5" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B22" s="4" t="inlineStr"/>
-      <c r="C22" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A22" s="4" t="n">
+        <v>43078</v>
+      </c>
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C22" s="4" t="inlineStr"/>
       <c r="D22" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E22" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao I</t>
         </is>
       </c>
-      <c r="E22" s="4" t="n">
+      <c r="F22" s="4" t="n">
         <v>133951</v>
       </c>
-      <c r="F22" s="4" t="inlineStr">
+      <c r="G22" s="4" t="inlineStr">
         <is>
           <t>Datu Paglas CS</t>
         </is>
       </c>
-      <c r="G22" s="4" t="inlineStr">
+      <c r="H22" s="4" t="inlineStr">
         <is>
           <t>DATU PAGLAS</t>
         </is>
       </c>
-      <c r="H22" s="4" t="inlineStr"/>
-      <c r="I22" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I22" s="4" t="inlineStr"/>
       <c r="J22" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="K22" s="4" t="inlineStr">
+      <c r="L22" s="4" t="inlineStr">
         <is>
           <t>1STY8CL</t>
         </is>
       </c>
-      <c r="L22" s="4" t="inlineStr">
+      <c r="M22" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M22" s="4" t="n">
+      <c r="N22" s="4" t="n">
         <v>20000000</v>
       </c>
-      <c r="N22" s="4" t="inlineStr"/>
       <c r="O22" s="4" t="inlineStr"/>
-      <c r="P22" s="4" t="inlineStr">
+      <c r="P22" s="4" t="inlineStr"/>
+      <c r="Q22" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" s="4" t="inlineStr"/>
+      <c r="R22" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S22" s="4" t="inlineStr"/>
       <c r="T22" s="4" t="inlineStr"/>
       <c r="U22" s="4" t="inlineStr"/>
@@ -2151,67 +2219,70 @@
       <c r="Z22" s="4" t="inlineStr"/>
       <c r="AA22" s="4" t="inlineStr"/>
       <c r="AB22" s="4" t="inlineStr"/>
-      <c r="AC22" s="5" t="n"/>
+      <c r="AC22" s="4" t="inlineStr"/>
+      <c r="AD22" s="5" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B23" s="4" t="inlineStr"/>
-      <c r="C23" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A23" s="4" t="n">
+        <v>43079</v>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C23" s="4" t="inlineStr"/>
       <c r="D23" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao I</t>
         </is>
       </c>
-      <c r="E23" s="4" t="inlineStr"/>
-      <c r="F23" s="4" t="inlineStr">
+      <c r="F23" s="4" t="inlineStr"/>
+      <c r="G23" s="4" t="inlineStr">
         <is>
           <t>Tocao - Madidis National High School</t>
         </is>
       </c>
-      <c r="G23" s="4" t="inlineStr">
+      <c r="H23" s="4" t="inlineStr">
         <is>
           <t>DATU PAGLAS</t>
         </is>
       </c>
-      <c r="H23" s="4" t="inlineStr"/>
-      <c r="I23" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I23" s="4" t="inlineStr"/>
       <c r="J23" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="K23" s="4" t="inlineStr">
+      <c r="L23" s="4" t="inlineStr">
         <is>
           <t>1STY8CL</t>
         </is>
       </c>
-      <c r="L23" s="4" t="inlineStr">
+      <c r="M23" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M23" s="4" t="n">
+      <c r="N23" s="4" t="n">
         <v>20000000</v>
       </c>
-      <c r="N23" s="4" t="inlineStr"/>
       <c r="O23" s="4" t="inlineStr"/>
-      <c r="P23" s="4" t="inlineStr">
+      <c r="P23" s="4" t="inlineStr"/>
+      <c r="Q23" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" s="4" t="inlineStr"/>
+      <c r="R23" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S23" s="4" t="inlineStr"/>
       <c r="T23" s="4" t="inlineStr"/>
       <c r="U23" s="4" t="inlineStr"/>
@@ -2222,67 +2293,70 @@
       <c r="Z23" s="4" t="inlineStr"/>
       <c r="AA23" s="4" t="inlineStr"/>
       <c r="AB23" s="4" t="inlineStr"/>
-      <c r="AC23" s="5" t="n"/>
+      <c r="AC23" s="4" t="inlineStr"/>
+      <c r="AD23" s="5" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B24" s="4" t="inlineStr"/>
-      <c r="C24" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A24" s="4" t="n">
+        <v>43080</v>
+      </c>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C24" s="4" t="inlineStr"/>
       <c r="D24" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="E24" s="4" t="inlineStr"/>
-      <c r="F24" s="4" t="inlineStr">
+      <c r="F24" s="4" t="inlineStr"/>
+      <c r="G24" s="4" t="inlineStr">
         <is>
           <t>Pura ES</t>
         </is>
       </c>
-      <c r="G24" s="4" t="inlineStr">
+      <c r="H24" s="4" t="inlineStr">
         <is>
           <t>DATU BLAH T. SINSUAT</t>
         </is>
       </c>
-      <c r="H24" s="4" t="inlineStr"/>
-      <c r="I24" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I24" s="4" t="inlineStr"/>
       <c r="J24" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K24" s="4" t="inlineStr">
+      <c r="L24" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L24" s="4" t="inlineStr">
+      <c r="M24" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M24" s="4" t="n">
+      <c r="N24" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N24" s="4" t="inlineStr"/>
       <c r="O24" s="4" t="inlineStr"/>
-      <c r="P24" s="4" t="inlineStr">
+      <c r="P24" s="4" t="inlineStr"/>
+      <c r="Q24" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q24" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" s="4" t="inlineStr"/>
+      <c r="R24" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S24" s="4" t="inlineStr"/>
       <c r="T24" s="4" t="inlineStr"/>
       <c r="U24" s="4" t="inlineStr"/>
@@ -2293,69 +2367,72 @@
       <c r="Z24" s="4" t="inlineStr"/>
       <c r="AA24" s="4" t="inlineStr"/>
       <c r="AB24" s="4" t="inlineStr"/>
-      <c r="AC24" s="5" t="n"/>
+      <c r="AC24" s="4" t="inlineStr"/>
+      <c r="AD24" s="5" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B25" s="4" t="inlineStr"/>
-      <c r="C25" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A25" s="4" t="n">
+        <v>43081</v>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C25" s="4" t="inlineStr"/>
       <c r="D25" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E25" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="E25" s="4" t="n">
+      <c r="F25" s="4" t="n">
         <v>216594</v>
       </c>
-      <c r="F25" s="4" t="inlineStr">
+      <c r="G25" s="4" t="inlineStr">
         <is>
           <t>Butilen Elementary School</t>
         </is>
       </c>
-      <c r="G25" s="4" t="inlineStr">
+      <c r="H25" s="4" t="inlineStr">
         <is>
           <t>KABUNTALAN (TUMBAO)</t>
         </is>
       </c>
-      <c r="H25" s="4" t="inlineStr"/>
-      <c r="I25" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I25" s="4" t="inlineStr"/>
       <c r="J25" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K25" s="4" t="inlineStr">
+      <c r="L25" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L25" s="4" t="inlineStr">
+      <c r="M25" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M25" s="4" t="n">
+      <c r="N25" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N25" s="4" t="inlineStr"/>
       <c r="O25" s="4" t="inlineStr"/>
-      <c r="P25" s="4" t="inlineStr">
+      <c r="P25" s="4" t="inlineStr"/>
+      <c r="Q25" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q25" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R25" s="4" t="inlineStr"/>
+      <c r="R25" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S25" s="4" t="inlineStr"/>
       <c r="T25" s="4" t="inlineStr"/>
       <c r="U25" s="4" t="inlineStr"/>
@@ -2366,69 +2443,72 @@
       <c r="Z25" s="4" t="inlineStr"/>
       <c r="AA25" s="4" t="inlineStr"/>
       <c r="AB25" s="4" t="inlineStr"/>
-      <c r="AC25" s="5" t="n"/>
+      <c r="AC25" s="4" t="inlineStr"/>
+      <c r="AD25" s="5" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B26" s="4" t="inlineStr"/>
-      <c r="C26" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A26" s="4" t="n">
+        <v>43082</v>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C26" s="4" t="inlineStr"/>
       <c r="D26" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E26" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="E26" s="4" t="n">
+      <c r="F26" s="4" t="n">
         <v>134033</v>
       </c>
-      <c r="F26" s="4" t="inlineStr">
+      <c r="G26" s="4" t="inlineStr">
         <is>
           <t>Maitong ES</t>
         </is>
       </c>
-      <c r="G26" s="4" t="inlineStr">
+      <c r="H26" s="4" t="inlineStr">
         <is>
           <t>KABUNTALAN (TUMBAO)</t>
         </is>
       </c>
-      <c r="H26" s="4" t="inlineStr"/>
-      <c r="I26" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I26" s="4" t="inlineStr"/>
       <c r="J26" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K26" s="4" t="inlineStr">
+      <c r="L26" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L26" s="4" t="inlineStr">
+      <c r="M26" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M26" s="4" t="n">
+      <c r="N26" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N26" s="4" t="inlineStr"/>
       <c r="O26" s="4" t="inlineStr"/>
-      <c r="P26" s="4" t="inlineStr">
+      <c r="P26" s="4" t="inlineStr"/>
+      <c r="Q26" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R26" s="4" t="inlineStr"/>
+      <c r="R26" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S26" s="4" t="inlineStr"/>
       <c r="T26" s="4" t="inlineStr"/>
       <c r="U26" s="4" t="inlineStr"/>
@@ -2439,67 +2519,70 @@
       <c r="Z26" s="4" t="inlineStr"/>
       <c r="AA26" s="4" t="inlineStr"/>
       <c r="AB26" s="4" t="inlineStr"/>
-      <c r="AC26" s="5" t="n"/>
+      <c r="AC26" s="4" t="inlineStr"/>
+      <c r="AD26" s="5" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B27" s="4" t="inlineStr"/>
-      <c r="C27" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A27" s="4" t="n">
+        <v>43083</v>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C27" s="4" t="inlineStr"/>
       <c r="D27" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="E27" s="4" t="inlineStr"/>
-      <c r="F27" s="4" t="inlineStr">
+      <c r="F27" s="4" t="inlineStr"/>
+      <c r="G27" s="4" t="inlineStr">
         <is>
           <t>Bayanga Norte ES</t>
         </is>
       </c>
-      <c r="G27" s="4" t="inlineStr">
+      <c r="H27" s="4" t="inlineStr">
         <is>
           <t>MATANOG</t>
         </is>
       </c>
-      <c r="H27" s="4" t="inlineStr"/>
-      <c r="I27" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I27" s="4" t="inlineStr"/>
       <c r="J27" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K27" s="4" t="inlineStr">
+      <c r="L27" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L27" s="4" t="inlineStr">
+      <c r="M27" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M27" s="4" t="n">
+      <c r="N27" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N27" s="4" t="inlineStr"/>
       <c r="O27" s="4" t="inlineStr"/>
-      <c r="P27" s="4" t="inlineStr">
+      <c r="P27" s="4" t="inlineStr"/>
+      <c r="Q27" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q27" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R27" s="4" t="inlineStr"/>
+      <c r="R27" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S27" s="4" t="inlineStr"/>
       <c r="T27" s="4" t="inlineStr"/>
       <c r="U27" s="4" t="inlineStr"/>
@@ -2510,69 +2593,72 @@
       <c r="Z27" s="4" t="inlineStr"/>
       <c r="AA27" s="4" t="inlineStr"/>
       <c r="AB27" s="4" t="inlineStr"/>
-      <c r="AC27" s="5" t="n"/>
+      <c r="AC27" s="4" t="inlineStr"/>
+      <c r="AD27" s="5" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B28" s="4" t="inlineStr"/>
-      <c r="C28" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A28" s="4" t="n">
+        <v>43084</v>
+      </c>
+      <c r="B28" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C28" s="4" t="inlineStr"/>
       <c r="D28" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E28" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="E28" s="4" t="n">
+      <c r="F28" s="4" t="n">
         <v>134158</v>
       </c>
-      <c r="F28" s="4" t="inlineStr">
+      <c r="G28" s="4" t="inlineStr">
         <is>
           <t>Alamada ES</t>
         </is>
       </c>
-      <c r="G28" s="4" t="inlineStr">
+      <c r="H28" s="4" t="inlineStr">
         <is>
           <t>SULTAN KUDARAT (NULING)</t>
         </is>
       </c>
-      <c r="H28" s="4" t="inlineStr"/>
-      <c r="I28" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I28" s="4" t="inlineStr"/>
       <c r="J28" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K28" s="4" t="inlineStr">
+      <c r="L28" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L28" s="4" t="inlineStr">
+      <c r="M28" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M28" s="4" t="n">
+      <c r="N28" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N28" s="4" t="inlineStr"/>
       <c r="O28" s="4" t="inlineStr"/>
-      <c r="P28" s="4" t="inlineStr">
+      <c r="P28" s="4" t="inlineStr"/>
+      <c r="Q28" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q28" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" s="4" t="inlineStr"/>
+      <c r="R28" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S28" s="4" t="inlineStr"/>
       <c r="T28" s="4" t="inlineStr"/>
       <c r="U28" s="4" t="inlineStr"/>
@@ -2583,69 +2669,72 @@
       <c r="Z28" s="4" t="inlineStr"/>
       <c r="AA28" s="4" t="inlineStr"/>
       <c r="AB28" s="4" t="inlineStr"/>
-      <c r="AC28" s="5" t="n"/>
+      <c r="AC28" s="4" t="inlineStr"/>
+      <c r="AD28" s="5" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B29" s="4" t="inlineStr"/>
-      <c r="C29" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A29" s="4" t="n">
+        <v>43085</v>
+      </c>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C29" s="4" t="inlineStr"/>
       <c r="D29" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E29" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="E29" s="4" t="n">
+      <c r="F29" s="4" t="n">
         <v>134143</v>
       </c>
-      <c r="F29" s="4" t="inlineStr">
+      <c r="G29" s="4" t="inlineStr">
         <is>
           <t>Ibotigen ES</t>
         </is>
       </c>
-      <c r="G29" s="4" t="inlineStr">
+      <c r="H29" s="4" t="inlineStr">
         <is>
           <t>SULTAN KUDARAT (NULING)</t>
         </is>
       </c>
-      <c r="H29" s="4" t="inlineStr"/>
-      <c r="I29" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I29" s="4" t="inlineStr"/>
       <c r="J29" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K29" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K29" s="4" t="inlineStr">
+      <c r="L29" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L29" s="4" t="inlineStr">
+      <c r="M29" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M29" s="4" t="n">
+      <c r="N29" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N29" s="4" t="inlineStr"/>
       <c r="O29" s="4" t="inlineStr"/>
-      <c r="P29" s="4" t="inlineStr">
+      <c r="P29" s="4" t="inlineStr"/>
+      <c r="Q29" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q29" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R29" s="4" t="inlineStr"/>
+      <c r="R29" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S29" s="4" t="inlineStr"/>
       <c r="T29" s="4" t="inlineStr"/>
       <c r="U29" s="4" t="inlineStr"/>
@@ -2656,67 +2745,70 @@
       <c r="Z29" s="4" t="inlineStr"/>
       <c r="AA29" s="4" t="inlineStr"/>
       <c r="AB29" s="4" t="inlineStr"/>
-      <c r="AC29" s="5" t="n"/>
+      <c r="AC29" s="4" t="inlineStr"/>
+      <c r="AD29" s="5" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B30" s="4" t="inlineStr"/>
-      <c r="C30" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A30" s="4" t="n">
+        <v>43086</v>
+      </c>
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C30" s="4" t="inlineStr"/>
       <c r="D30" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E30" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="E30" s="4" t="inlineStr"/>
-      <c r="F30" s="4" t="inlineStr">
+      <c r="F30" s="4" t="inlineStr"/>
+      <c r="G30" s="4" t="inlineStr">
         <is>
           <t>Inawan ES</t>
         </is>
       </c>
-      <c r="G30" s="4" t="inlineStr">
+      <c r="H30" s="4" t="inlineStr">
         <is>
           <t>SULTAN KUDARAT (NULING)</t>
         </is>
       </c>
-      <c r="H30" s="4" t="inlineStr"/>
-      <c r="I30" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I30" s="4" t="inlineStr"/>
       <c r="J30" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K30" s="4" t="inlineStr">
+      <c r="L30" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L30" s="4" t="inlineStr">
+      <c r="M30" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M30" s="4" t="n">
+      <c r="N30" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N30" s="4" t="inlineStr"/>
       <c r="O30" s="4" t="inlineStr"/>
-      <c r="P30" s="4" t="inlineStr">
+      <c r="P30" s="4" t="inlineStr"/>
+      <c r="Q30" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q30" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" s="4" t="inlineStr"/>
+      <c r="R30" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S30" s="4" t="inlineStr"/>
       <c r="T30" s="4" t="inlineStr"/>
       <c r="U30" s="4" t="inlineStr"/>
@@ -2727,69 +2819,72 @@
       <c r="Z30" s="4" t="inlineStr"/>
       <c r="AA30" s="4" t="inlineStr"/>
       <c r="AB30" s="4" t="inlineStr"/>
-      <c r="AC30" s="5" t="n"/>
+      <c r="AC30" s="4" t="inlineStr"/>
+      <c r="AD30" s="5" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B31" s="4" t="inlineStr"/>
-      <c r="C31" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A31" s="4" t="n">
+        <v>43087</v>
+      </c>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C31" s="4" t="inlineStr"/>
       <c r="D31" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E31" s="4" t="inlineStr">
+        <is>
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="E31" s="4" t="n">
+      <c r="F31" s="4" t="n">
         <v>134237</v>
       </c>
-      <c r="F31" s="4" t="inlineStr">
+      <c r="G31" s="4" t="inlineStr">
         <is>
           <t>Ranao Pilayan ES</t>
         </is>
       </c>
-      <c r="G31" s="4" t="inlineStr">
+      <c r="H31" s="4" t="inlineStr">
         <is>
           <t>UPI</t>
         </is>
       </c>
-      <c r="H31" s="4" t="inlineStr"/>
-      <c r="I31" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I31" s="4" t="inlineStr"/>
       <c r="J31" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K31" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K31" s="4" t="inlineStr">
+      <c r="L31" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L31" s="4" t="inlineStr">
+      <c r="M31" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M31" s="4" t="n">
+      <c r="N31" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N31" s="4" t="inlineStr"/>
       <c r="O31" s="4" t="inlineStr"/>
-      <c r="P31" s="4" t="inlineStr">
+      <c r="P31" s="4" t="inlineStr"/>
+      <c r="Q31" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q31" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R31" s="4" t="inlineStr"/>
+      <c r="R31" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S31" s="4" t="inlineStr"/>
       <c r="T31" s="4" t="inlineStr"/>
       <c r="U31" s="4" t="inlineStr"/>
@@ -2800,69 +2895,72 @@
       <c r="Z31" s="4" t="inlineStr"/>
       <c r="AA31" s="4" t="inlineStr"/>
       <c r="AB31" s="4" t="inlineStr"/>
-      <c r="AC31" s="5" t="n"/>
+      <c r="AC31" s="4" t="inlineStr"/>
+      <c r="AD31" s="5" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B32" s="4" t="inlineStr"/>
-      <c r="C32" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A32" s="4" t="n">
+        <v>43088</v>
+      </c>
+      <c r="B32" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C32" s="4" t="inlineStr"/>
       <c r="D32" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E32" s="4" t="inlineStr">
+        <is>
           <t>Marawi City</t>
         </is>
       </c>
-      <c r="E32" s="4" t="n">
+      <c r="F32" s="4" t="n">
         <v>134934</v>
       </c>
-      <c r="F32" s="4" t="inlineStr">
+      <c r="G32" s="4" t="inlineStr">
         <is>
           <t>Amai Pakpak CES</t>
         </is>
       </c>
-      <c r="G32" s="4" t="inlineStr">
+      <c r="H32" s="4" t="inlineStr">
         <is>
           <t>MARAWI CITY</t>
         </is>
       </c>
-      <c r="H32" s="4" t="inlineStr"/>
-      <c r="I32" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I32" s="4" t="inlineStr"/>
       <c r="J32" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K32" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="K32" s="4" t="inlineStr">
+      <c r="L32" s="4" t="inlineStr">
         <is>
           <t>3STY12CL</t>
         </is>
       </c>
-      <c r="L32" s="4" t="inlineStr">
+      <c r="M32" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M32" s="4" t="n">
+      <c r="N32" s="4" t="n">
         <v>42000000</v>
       </c>
-      <c r="N32" s="4" t="inlineStr"/>
       <c r="O32" s="4" t="inlineStr"/>
-      <c r="P32" s="4" t="inlineStr">
+      <c r="P32" s="4" t="inlineStr"/>
+      <c r="Q32" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q32" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" s="4" t="inlineStr"/>
+      <c r="R32" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S32" s="4" t="inlineStr"/>
       <c r="T32" s="4" t="inlineStr"/>
       <c r="U32" s="4" t="inlineStr"/>
@@ -2873,69 +2971,72 @@
       <c r="Z32" s="4" t="inlineStr"/>
       <c r="AA32" s="4" t="inlineStr"/>
       <c r="AB32" s="4" t="inlineStr"/>
-      <c r="AC32" s="5" t="n"/>
+      <c r="AC32" s="4" t="inlineStr"/>
+      <c r="AD32" s="5" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B33" s="4" t="inlineStr"/>
-      <c r="C33" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A33" s="4" t="n">
+        <v>43089</v>
+      </c>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C33" s="4" t="inlineStr"/>
       <c r="D33" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E33" s="4" t="inlineStr">
+        <is>
           <t>Sulu</t>
         </is>
       </c>
-      <c r="E33" s="4" t="n">
+      <c r="F33" s="4" t="n">
         <v>134444</v>
       </c>
-      <c r="F33" s="4" t="inlineStr">
+      <c r="G33" s="4" t="inlineStr">
         <is>
           <t>Bualoh Lipid ES</t>
         </is>
       </c>
-      <c r="G33" s="4" t="inlineStr">
+      <c r="H33" s="4" t="inlineStr">
         <is>
           <t>MAIMBUNG</t>
         </is>
       </c>
-      <c r="H33" s="4" t="inlineStr"/>
-      <c r="I33" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I33" s="4" t="inlineStr"/>
       <c r="J33" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="K33" s="4" t="inlineStr">
+      <c r="L33" s="4" t="inlineStr">
         <is>
           <t>1STY4CL</t>
         </is>
       </c>
-      <c r="L33" s="4" t="inlineStr">
+      <c r="M33" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M33" s="4" t="n">
+      <c r="N33" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N33" s="4" t="inlineStr"/>
       <c r="O33" s="4" t="inlineStr"/>
-      <c r="P33" s="4" t="inlineStr">
+      <c r="P33" s="4" t="inlineStr"/>
+      <c r="Q33" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q33" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R33" s="4" t="inlineStr"/>
+      <c r="R33" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S33" s="4" t="inlineStr"/>
       <c r="T33" s="4" t="inlineStr"/>
       <c r="U33" s="4" t="inlineStr"/>
@@ -2946,67 +3047,70 @@
       <c r="Z33" s="4" t="inlineStr"/>
       <c r="AA33" s="4" t="inlineStr"/>
       <c r="AB33" s="4" t="inlineStr"/>
-      <c r="AC33" s="5" t="n"/>
+      <c r="AC33" s="4" t="inlineStr"/>
+      <c r="AD33" s="5" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B34" s="4" t="inlineStr"/>
-      <c r="C34" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A34" s="4" t="n">
+        <v>43090</v>
+      </c>
+      <c r="B34" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C34" s="4" t="inlineStr"/>
       <c r="D34" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E34" s="4" t="inlineStr">
+        <is>
           <t>Sulu</t>
         </is>
       </c>
-      <c r="E34" s="4" t="inlineStr"/>
-      <c r="F34" s="4" t="inlineStr">
+      <c r="F34" s="4" t="inlineStr"/>
+      <c r="G34" s="4" t="inlineStr">
         <is>
           <t>Sultan Jamalul Kiram Central High School</t>
         </is>
       </c>
-      <c r="G34" s="4" t="inlineStr">
+      <c r="H34" s="4" t="inlineStr">
         <is>
           <t>MAIMBUNG</t>
         </is>
       </c>
-      <c r="H34" s="4" t="inlineStr"/>
-      <c r="I34" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I34" s="4" t="inlineStr"/>
       <c r="J34" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="K34" s="4" t="inlineStr">
+      <c r="L34" s="4" t="inlineStr">
         <is>
           <t>2STY10CL</t>
         </is>
       </c>
-      <c r="L34" s="4" t="inlineStr">
+      <c r="M34" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M34" s="4" t="n">
+      <c r="N34" s="4" t="n">
         <v>40000000</v>
       </c>
-      <c r="N34" s="4" t="inlineStr"/>
       <c r="O34" s="4" t="inlineStr"/>
-      <c r="P34" s="4" t="inlineStr">
+      <c r="P34" s="4" t="inlineStr"/>
+      <c r="Q34" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q34" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R34" s="4" t="inlineStr"/>
+      <c r="R34" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S34" s="4" t="inlineStr"/>
       <c r="T34" s="4" t="inlineStr"/>
       <c r="U34" s="4" t="inlineStr"/>
@@ -3017,67 +3121,70 @@
       <c r="Z34" s="4" t="inlineStr"/>
       <c r="AA34" s="4" t="inlineStr"/>
       <c r="AB34" s="4" t="inlineStr"/>
-      <c r="AC34" s="5" t="n"/>
+      <c r="AC34" s="4" t="inlineStr"/>
+      <c r="AD34" s="5" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B35" s="4" t="inlineStr"/>
-      <c r="C35" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A35" s="4" t="n">
+        <v>43091</v>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C35" s="4" t="inlineStr"/>
       <c r="D35" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E35" s="4" t="inlineStr">
+        <is>
           <t>Sulu</t>
         </is>
       </c>
-      <c r="E35" s="4" t="inlineStr"/>
-      <c r="F35" s="4" t="inlineStr">
+      <c r="F35" s="4" t="inlineStr"/>
+      <c r="G35" s="4" t="inlineStr">
         <is>
           <t>Patikul NHS - Extension</t>
         </is>
       </c>
-      <c r="G35" s="4" t="inlineStr">
+      <c r="H35" s="4" t="inlineStr">
         <is>
           <t>PATIKUL</t>
         </is>
       </c>
-      <c r="H35" s="4" t="inlineStr"/>
-      <c r="I35" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I35" s="4" t="inlineStr"/>
       <c r="J35" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K35" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="K35" s="4" t="inlineStr">
+      <c r="L35" s="4" t="inlineStr">
         <is>
           <t>1STY4CL</t>
         </is>
       </c>
-      <c r="L35" s="4" t="inlineStr">
+      <c r="M35" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M35" s="4" t="n">
+      <c r="N35" s="4" t="n">
         <v>10000000</v>
       </c>
-      <c r="N35" s="4" t="inlineStr"/>
       <c r="O35" s="4" t="inlineStr"/>
-      <c r="P35" s="4" t="inlineStr">
+      <c r="P35" s="4" t="inlineStr"/>
+      <c r="Q35" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q35" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R35" s="4" t="inlineStr"/>
+      <c r="R35" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S35" s="4" t="inlineStr"/>
       <c r="T35" s="4" t="inlineStr"/>
       <c r="U35" s="4" t="inlineStr"/>
@@ -3088,69 +3195,72 @@
       <c r="Z35" s="4" t="inlineStr"/>
       <c r="AA35" s="4" t="inlineStr"/>
       <c r="AB35" s="4" t="inlineStr"/>
-      <c r="AC35" s="5" t="n"/>
+      <c r="AC35" s="4" t="inlineStr"/>
+      <c r="AD35" s="5" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B36" s="4" t="inlineStr"/>
-      <c r="C36" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A36" s="4" t="n">
+        <v>43092</v>
+      </c>
+      <c r="B36" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C36" s="4" t="inlineStr"/>
       <c r="D36" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E36" s="4" t="inlineStr">
+        <is>
           <t>Sulu</t>
         </is>
       </c>
-      <c r="E36" s="4" t="n">
+      <c r="F36" s="4" t="n">
         <v>134416</v>
       </c>
-      <c r="F36" s="4" t="inlineStr">
+      <c r="G36" s="4" t="inlineStr">
         <is>
           <t>Camp Andres CES</t>
         </is>
       </c>
-      <c r="G36" s="4" t="inlineStr">
+      <c r="H36" s="4" t="inlineStr">
         <is>
           <t>LUUK</t>
         </is>
       </c>
-      <c r="H36" s="4" t="inlineStr"/>
-      <c r="I36" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I36" s="4" t="inlineStr"/>
       <c r="J36" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K36" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="K36" s="4" t="inlineStr">
+      <c r="L36" s="4" t="inlineStr">
         <is>
           <t>3STY12CL</t>
         </is>
       </c>
-      <c r="L36" s="4" t="inlineStr">
+      <c r="M36" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M36" s="4" t="n">
+      <c r="N36" s="4" t="n">
         <v>40000000</v>
       </c>
-      <c r="N36" s="4" t="inlineStr"/>
       <c r="O36" s="4" t="inlineStr"/>
-      <c r="P36" s="4" t="inlineStr">
+      <c r="P36" s="4" t="inlineStr"/>
+      <c r="Q36" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q36" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R36" s="4" t="inlineStr"/>
+      <c r="R36" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S36" s="4" t="inlineStr"/>
       <c r="T36" s="4" t="inlineStr"/>
       <c r="U36" s="4" t="inlineStr"/>
@@ -3161,69 +3271,72 @@
       <c r="Z36" s="4" t="inlineStr"/>
       <c r="AA36" s="4" t="inlineStr"/>
       <c r="AB36" s="4" t="inlineStr"/>
-      <c r="AC36" s="5" t="n"/>
+      <c r="AC36" s="4" t="inlineStr"/>
+      <c r="AD36" s="5" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B37" s="4" t="inlineStr"/>
-      <c r="C37" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A37" s="4" t="n">
+        <v>43093</v>
+      </c>
+      <c r="B37" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C37" s="4" t="inlineStr"/>
       <c r="D37" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E37" s="4" t="inlineStr">
+        <is>
           <t>Sulu</t>
         </is>
       </c>
-      <c r="E37" s="4" t="n">
+      <c r="F37" s="4" t="n">
         <v>252514</v>
       </c>
-      <c r="F37" s="4" t="inlineStr">
+      <c r="G37" s="4" t="inlineStr">
         <is>
           <t>Sapang PS</t>
         </is>
       </c>
-      <c r="G37" s="4" t="inlineStr">
+      <c r="H37" s="4" t="inlineStr">
         <is>
           <t>LUUK</t>
         </is>
       </c>
-      <c r="H37" s="4" t="inlineStr"/>
-      <c r="I37" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I37" s="4" t="inlineStr"/>
       <c r="J37" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K37" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="K37" s="4" t="inlineStr">
+      <c r="L37" s="4" t="inlineStr">
         <is>
           <t>1STY3CL</t>
         </is>
       </c>
-      <c r="L37" s="4" t="inlineStr">
+      <c r="M37" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M37" s="4" t="n">
+      <c r="N37" s="4" t="n">
         <v>7329687.55</v>
       </c>
-      <c r="N37" s="4" t="inlineStr"/>
       <c r="O37" s="4" t="inlineStr"/>
-      <c r="P37" s="4" t="inlineStr">
+      <c r="P37" s="4" t="inlineStr"/>
+      <c r="Q37" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q37" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R37" s="4" t="inlineStr"/>
+      <c r="R37" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S37" s="4" t="inlineStr"/>
       <c r="T37" s="4" t="inlineStr"/>
       <c r="U37" s="4" t="inlineStr"/>
@@ -3234,69 +3347,72 @@
       <c r="Z37" s="4" t="inlineStr"/>
       <c r="AA37" s="4" t="inlineStr"/>
       <c r="AB37" s="4" t="inlineStr"/>
-      <c r="AC37" s="5" t="n"/>
+      <c r="AC37" s="4" t="inlineStr"/>
+      <c r="AD37" s="5" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B38" s="4" t="inlineStr"/>
-      <c r="C38" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A38" s="4" t="n">
+        <v>43094</v>
+      </c>
+      <c r="B38" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C38" s="4" t="inlineStr"/>
       <c r="D38" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E38" s="4" t="inlineStr">
+        <is>
           <t>Sulu</t>
         </is>
       </c>
-      <c r="E38" s="4" t="n">
+      <c r="F38" s="4" t="n">
         <v>134439</v>
       </c>
-      <c r="F38" s="4" t="inlineStr">
+      <c r="G38" s="4" t="inlineStr">
         <is>
           <t>Tandu Bato ES</t>
         </is>
       </c>
-      <c r="G38" s="4" t="inlineStr">
+      <c r="H38" s="4" t="inlineStr">
         <is>
           <t>LUUK</t>
         </is>
       </c>
-      <c r="H38" s="4" t="inlineStr"/>
-      <c r="I38" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I38" s="4" t="inlineStr"/>
       <c r="J38" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="K38" s="4" t="inlineStr">
+      <c r="L38" s="4" t="inlineStr">
         <is>
           <t>1STY3CL</t>
         </is>
       </c>
-      <c r="L38" s="4" t="inlineStr">
+      <c r="M38" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M38" s="4" t="n">
+      <c r="N38" s="4" t="n">
         <v>7329687.55</v>
       </c>
-      <c r="N38" s="4" t="inlineStr"/>
       <c r="O38" s="4" t="inlineStr"/>
-      <c r="P38" s="4" t="inlineStr">
+      <c r="P38" s="4" t="inlineStr"/>
+      <c r="Q38" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q38" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R38" s="4" t="inlineStr"/>
+      <c r="R38" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S38" s="4" t="inlineStr"/>
       <c r="T38" s="4" t="inlineStr"/>
       <c r="U38" s="4" t="inlineStr"/>
@@ -3307,69 +3423,72 @@
       <c r="Z38" s="4" t="inlineStr"/>
       <c r="AA38" s="4" t="inlineStr"/>
       <c r="AB38" s="4" t="inlineStr"/>
-      <c r="AC38" s="5" t="n"/>
+      <c r="AC38" s="4" t="inlineStr"/>
+      <c r="AD38" s="5" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B39" s="4" t="inlineStr"/>
-      <c r="C39" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A39" s="4" t="n">
+        <v>43095</v>
+      </c>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C39" s="4" t="inlineStr"/>
       <c r="D39" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E39" s="4" t="inlineStr">
+        <is>
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="E39" s="4" t="n">
+      <c r="F39" s="4" t="n">
         <v>134902</v>
       </c>
-      <c r="F39" s="4" t="inlineStr">
+      <c r="G39" s="4" t="inlineStr">
         <is>
           <t>Datu Halun Laboratory School</t>
         </is>
       </c>
-      <c r="G39" s="4" t="inlineStr">
+      <c r="H39" s="4" t="inlineStr">
         <is>
           <t>BONGAO</t>
         </is>
       </c>
-      <c r="H39" s="4" t="inlineStr"/>
-      <c r="I39" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I39" s="4" t="inlineStr"/>
       <c r="J39" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K39" s="4" t="inlineStr">
+      <c r="L39" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L39" s="4" t="inlineStr">
+      <c r="M39" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M39" s="4" t="n">
+      <c r="N39" s="4" t="n">
         <v>5670312.45</v>
       </c>
-      <c r="N39" s="4" t="inlineStr"/>
       <c r="O39" s="4" t="inlineStr"/>
-      <c r="P39" s="4" t="inlineStr">
+      <c r="P39" s="4" t="inlineStr"/>
+      <c r="Q39" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q39" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R39" s="4" t="inlineStr"/>
+      <c r="R39" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S39" s="4" t="inlineStr"/>
       <c r="T39" s="4" t="inlineStr"/>
       <c r="U39" s="4" t="inlineStr"/>
@@ -3380,69 +3499,72 @@
       <c r="Z39" s="4" t="inlineStr"/>
       <c r="AA39" s="4" t="inlineStr"/>
       <c r="AB39" s="4" t="inlineStr"/>
-      <c r="AC39" s="5" t="n"/>
+      <c r="AC39" s="4" t="inlineStr"/>
+      <c r="AD39" s="5" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B40" s="4" t="inlineStr"/>
-      <c r="C40" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A40" s="4" t="n">
+        <v>43096</v>
+      </c>
+      <c r="B40" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C40" s="4" t="inlineStr"/>
       <c r="D40" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E40" s="4" t="inlineStr">
+        <is>
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="E40" s="4" t="n">
+      <c r="F40" s="4" t="n">
         <v>134716</v>
       </c>
-      <c r="F40" s="4" t="inlineStr">
+      <c r="G40" s="4" t="inlineStr">
         <is>
           <t>Lamion Walking (Main) ES</t>
         </is>
       </c>
-      <c r="G40" s="4" t="inlineStr">
+      <c r="H40" s="4" t="inlineStr">
         <is>
           <t>BONGAO</t>
         </is>
       </c>
-      <c r="H40" s="4" t="inlineStr"/>
-      <c r="I40" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I40" s="4" t="inlineStr"/>
       <c r="J40" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K40" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K40" s="4" t="inlineStr">
+      <c r="L40" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L40" s="4" t="inlineStr">
+      <c r="M40" s="4" t="inlineStr">
         <is>
           <t>BATCH 2</t>
         </is>
       </c>
-      <c r="M40" s="4" t="n">
+      <c r="N40" s="4" t="n">
         <v>5670312.45</v>
       </c>
-      <c r="N40" s="4" t="inlineStr"/>
       <c r="O40" s="4" t="inlineStr"/>
-      <c r="P40" s="4" t="inlineStr">
+      <c r="P40" s="4" t="inlineStr"/>
+      <c r="Q40" s="4" t="inlineStr">
         <is>
           <t>Ongoing</t>
         </is>
       </c>
-      <c r="Q40" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R40" s="4" t="inlineStr"/>
+      <c r="R40" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S40" s="4" t="inlineStr"/>
       <c r="T40" s="4" t="inlineStr"/>
       <c r="U40" s="4" t="inlineStr"/>
@@ -3453,69 +3575,72 @@
       <c r="Z40" s="4" t="inlineStr"/>
       <c r="AA40" s="4" t="inlineStr"/>
       <c r="AB40" s="4" t="inlineStr"/>
-      <c r="AC40" s="5" t="n"/>
+      <c r="AC40" s="4" t="inlineStr"/>
+      <c r="AD40" s="5" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B41" s="4" t="inlineStr"/>
-      <c r="C41" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A41" s="4" t="n">
+        <v>43097</v>
+      </c>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C41" s="4" t="inlineStr"/>
       <c r="D41" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E41" s="4" t="inlineStr">
+        <is>
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="E41" s="4" t="n">
+      <c r="F41" s="4" t="n">
         <v>305066</v>
       </c>
-      <c r="F41" s="4" t="inlineStr">
+      <c r="G41" s="4" t="inlineStr">
         <is>
           <t>Tawi Tawi SAT</t>
         </is>
       </c>
-      <c r="G41" s="4" t="inlineStr">
+      <c r="H41" s="4" t="inlineStr">
         <is>
           <t>BONGAO</t>
         </is>
       </c>
-      <c r="H41" s="4" t="inlineStr"/>
-      <c r="I41" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I41" s="4" t="inlineStr"/>
       <c r="J41" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K41" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K41" s="4" t="inlineStr">
+      <c r="L41" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L41" s="4" t="inlineStr">
+      <c r="M41" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M41" s="4" t="n">
+      <c r="N41" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N41" s="4" t="inlineStr"/>
       <c r="O41" s="4" t="inlineStr"/>
-      <c r="P41" s="4" t="inlineStr">
+      <c r="P41" s="4" t="inlineStr"/>
+      <c r="Q41" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q41" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" s="4" t="inlineStr"/>
+      <c r="R41" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S41" s="4" t="inlineStr"/>
       <c r="T41" s="4" t="inlineStr"/>
       <c r="U41" s="4" t="inlineStr"/>
@@ -3526,69 +3651,72 @@
       <c r="Z41" s="4" t="inlineStr"/>
       <c r="AA41" s="4" t="inlineStr"/>
       <c r="AB41" s="4" t="inlineStr"/>
-      <c r="AC41" s="5" t="n"/>
+      <c r="AC41" s="4" t="inlineStr"/>
+      <c r="AD41" s="5" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B42" s="4" t="inlineStr"/>
-      <c r="C42" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A42" s="4" t="n">
+        <v>43098</v>
+      </c>
+      <c r="B42" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C42" s="4" t="inlineStr"/>
       <c r="D42" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E42" s="4" t="inlineStr">
+        <is>
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="E42" s="4" t="n">
+      <c r="F42" s="4" t="n">
         <v>305065</v>
       </c>
-      <c r="F42" s="4" t="inlineStr">
+      <c r="G42" s="4" t="inlineStr">
         <is>
           <t>Tawi-Tawi School of Fisheries</t>
         </is>
       </c>
-      <c r="G42" s="4" t="inlineStr">
+      <c r="H42" s="4" t="inlineStr">
         <is>
           <t>BONGAO</t>
         </is>
       </c>
-      <c r="H42" s="4" t="inlineStr"/>
-      <c r="I42" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I42" s="4" t="inlineStr"/>
       <c r="J42" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K42" s="4" t="inlineStr">
+      <c r="L42" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L42" s="4" t="inlineStr">
+      <c r="M42" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M42" s="4" t="n">
+      <c r="N42" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N42" s="4" t="inlineStr"/>
       <c r="O42" s="4" t="inlineStr"/>
-      <c r="P42" s="4" t="inlineStr">
+      <c r="P42" s="4" t="inlineStr"/>
+      <c r="Q42" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q42" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" s="4" t="inlineStr"/>
+      <c r="R42" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S42" s="4" t="inlineStr"/>
       <c r="T42" s="4" t="inlineStr"/>
       <c r="U42" s="4" t="inlineStr"/>
@@ -3599,69 +3727,72 @@
       <c r="Z42" s="4" t="inlineStr"/>
       <c r="AA42" s="4" t="inlineStr"/>
       <c r="AB42" s="4" t="inlineStr"/>
-      <c r="AC42" s="5" t="n"/>
+      <c r="AC42" s="4" t="inlineStr"/>
+      <c r="AD42" s="5" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B43" s="4" t="inlineStr"/>
-      <c r="C43" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A43" s="4" t="n">
+        <v>43099</v>
+      </c>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C43" s="4" t="inlineStr"/>
       <c r="D43" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E43" s="4" t="inlineStr">
+        <is>
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="E43" s="4" t="n">
+      <c r="F43" s="4" t="n">
         <v>134886</v>
       </c>
-      <c r="F43" s="4" t="inlineStr">
+      <c r="G43" s="4" t="inlineStr">
         <is>
           <t>Campo Muslim Primary School</t>
         </is>
       </c>
-      <c r="G43" s="4" t="inlineStr">
+      <c r="H43" s="4" t="inlineStr">
         <is>
           <t>LANGUYAN</t>
         </is>
       </c>
-      <c r="H43" s="4" t="inlineStr"/>
-      <c r="I43" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I43" s="4" t="inlineStr"/>
       <c r="J43" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K43" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K43" s="4" t="inlineStr">
+      <c r="L43" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L43" s="4" t="inlineStr">
+      <c r="M43" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M43" s="4" t="n">
+      <c r="N43" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N43" s="4" t="inlineStr"/>
       <c r="O43" s="4" t="inlineStr"/>
-      <c r="P43" s="4" t="inlineStr">
+      <c r="P43" s="4" t="inlineStr"/>
+      <c r="Q43" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q43" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R43" s="4" t="inlineStr"/>
+      <c r="R43" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S43" s="4" t="inlineStr"/>
       <c r="T43" s="4" t="inlineStr"/>
       <c r="U43" s="4" t="inlineStr"/>
@@ -3672,67 +3803,70 @@
       <c r="Z43" s="4" t="inlineStr"/>
       <c r="AA43" s="4" t="inlineStr"/>
       <c r="AB43" s="4" t="inlineStr"/>
-      <c r="AC43" s="5" t="n"/>
+      <c r="AC43" s="4" t="inlineStr"/>
+      <c r="AD43" s="5" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B44" s="4" t="inlineStr"/>
-      <c r="C44" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A44" s="4" t="n">
+        <v>43100</v>
+      </c>
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C44" s="4" t="inlineStr"/>
       <c r="D44" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E44" s="4" t="inlineStr">
+        <is>
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="E44" s="4" t="inlineStr"/>
-      <c r="F44" s="4" t="inlineStr">
+      <c r="F44" s="4" t="inlineStr"/>
+      <c r="G44" s="4" t="inlineStr">
         <is>
           <t>Lupah Pula CS</t>
         </is>
       </c>
-      <c r="G44" s="4" t="inlineStr">
+      <c r="H44" s="4" t="inlineStr">
         <is>
           <t>MAPUN (CAGAYAN DE TAWI-TAWI)</t>
         </is>
       </c>
-      <c r="H44" s="4" t="inlineStr"/>
-      <c r="I44" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I44" s="4" t="inlineStr"/>
       <c r="J44" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K44" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K44" s="4" t="inlineStr">
+      <c r="L44" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L44" s="4" t="inlineStr">
+      <c r="M44" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M44" s="4" t="n">
+      <c r="N44" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N44" s="4" t="inlineStr"/>
       <c r="O44" s="4" t="inlineStr"/>
-      <c r="P44" s="4" t="inlineStr">
+      <c r="P44" s="4" t="inlineStr"/>
+      <c r="Q44" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q44" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R44" s="4" t="inlineStr"/>
+      <c r="R44" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S44" s="4" t="inlineStr"/>
       <c r="T44" s="4" t="inlineStr"/>
       <c r="U44" s="4" t="inlineStr"/>
@@ -3743,69 +3877,72 @@
       <c r="Z44" s="4" t="inlineStr"/>
       <c r="AA44" s="4" t="inlineStr"/>
       <c r="AB44" s="4" t="inlineStr"/>
-      <c r="AC44" s="5" t="n"/>
+      <c r="AC44" s="4" t="inlineStr"/>
+      <c r="AD44" s="5" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B45" s="4" t="inlineStr"/>
-      <c r="C45" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A45" s="4" t="n">
+        <v>43101</v>
+      </c>
+      <c r="B45" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C45" s="4" t="inlineStr"/>
       <c r="D45" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="E45" s="4" t="n">
+      <c r="F45" s="4" t="n">
         <v>305070</v>
       </c>
-      <c r="F45" s="4" t="inlineStr">
+      <c r="G45" s="4" t="inlineStr">
         <is>
           <t>UMMAT NHS</t>
         </is>
       </c>
-      <c r="G45" s="4" t="inlineStr">
+      <c r="H45" s="4" t="inlineStr">
         <is>
           <t>SIMUNUL</t>
         </is>
       </c>
-      <c r="H45" s="4" t="inlineStr"/>
-      <c r="I45" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I45" s="4" t="inlineStr"/>
       <c r="J45" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K45" s="4" t="inlineStr">
+      <c r="L45" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L45" s="4" t="inlineStr">
+      <c r="M45" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M45" s="4" t="n">
+      <c r="N45" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N45" s="4" t="inlineStr"/>
       <c r="O45" s="4" t="inlineStr"/>
-      <c r="P45" s="4" t="inlineStr">
+      <c r="P45" s="4" t="inlineStr"/>
+      <c r="Q45" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q45" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R45" s="4" t="inlineStr"/>
+      <c r="R45" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S45" s="4" t="inlineStr"/>
       <c r="T45" s="4" t="inlineStr"/>
       <c r="U45" s="4" t="inlineStr"/>
@@ -3816,69 +3953,72 @@
       <c r="Z45" s="4" t="inlineStr"/>
       <c r="AA45" s="4" t="inlineStr"/>
       <c r="AB45" s="4" t="inlineStr"/>
-      <c r="AC45" s="5" t="n"/>
+      <c r="AC45" s="4" t="inlineStr"/>
+      <c r="AD45" s="5" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B46" s="4" t="inlineStr"/>
-      <c r="C46" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A46" s="4" t="n">
+        <v>43102</v>
+      </c>
+      <c r="B46" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C46" s="4" t="inlineStr"/>
       <c r="D46" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E46" s="4" t="inlineStr">
+        <is>
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="E46" s="4" t="n">
+      <c r="F46" s="4" t="n">
         <v>134842</v>
       </c>
-      <c r="F46" s="4" t="inlineStr">
+      <c r="G46" s="4" t="inlineStr">
         <is>
           <t>Datu Halun CES</t>
         </is>
       </c>
-      <c r="G46" s="4" t="inlineStr">
+      <c r="H46" s="4" t="inlineStr">
         <is>
           <t>SITANGKAI</t>
         </is>
       </c>
-      <c r="H46" s="4" t="inlineStr"/>
-      <c r="I46" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I46" s="4" t="inlineStr"/>
       <c r="J46" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K46" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K46" s="4" t="inlineStr">
+      <c r="L46" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L46" s="4" t="inlineStr">
+      <c r="M46" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M46" s="4" t="n">
+      <c r="N46" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N46" s="4" t="inlineStr"/>
       <c r="O46" s="4" t="inlineStr"/>
-      <c r="P46" s="4" t="inlineStr">
+      <c r="P46" s="4" t="inlineStr"/>
+      <c r="Q46" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q46" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R46" s="4" t="inlineStr"/>
+      <c r="R46" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S46" s="4" t="inlineStr"/>
       <c r="T46" s="4" t="inlineStr"/>
       <c r="U46" s="4" t="inlineStr"/>
@@ -3889,69 +4029,72 @@
       <c r="Z46" s="4" t="inlineStr"/>
       <c r="AA46" s="4" t="inlineStr"/>
       <c r="AB46" s="4" t="inlineStr"/>
-      <c r="AC46" s="5" t="n"/>
+      <c r="AC46" s="4" t="inlineStr"/>
+      <c r="AD46" s="5" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B47" s="4" t="inlineStr"/>
-      <c r="C47" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A47" s="4" t="n">
+        <v>43103</v>
+      </c>
+      <c r="B47" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C47" s="4" t="inlineStr"/>
       <c r="D47" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E47" s="4" t="inlineStr">
+        <is>
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="E47" s="4" t="n">
+      <c r="F47" s="4" t="n">
         <v>134848</v>
       </c>
-      <c r="F47" s="4" t="inlineStr">
+      <c r="G47" s="4" t="inlineStr">
         <is>
           <t>Tongusong ES</t>
         </is>
       </c>
-      <c r="G47" s="4" t="inlineStr">
+      <c r="H47" s="4" t="inlineStr">
         <is>
           <t>SITANGKAI</t>
         </is>
       </c>
-      <c r="H47" s="4" t="inlineStr"/>
-      <c r="I47" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I47" s="4" t="inlineStr"/>
       <c r="J47" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K47" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K47" s="4" t="inlineStr">
+      <c r="L47" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L47" s="4" t="inlineStr">
+      <c r="M47" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M47" s="4" t="n">
+      <c r="N47" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N47" s="4" t="inlineStr"/>
       <c r="O47" s="4" t="inlineStr"/>
-      <c r="P47" s="4" t="inlineStr">
+      <c r="P47" s="4" t="inlineStr"/>
+      <c r="Q47" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q47" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R47" s="4" t="inlineStr"/>
+      <c r="R47" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S47" s="4" t="inlineStr"/>
       <c r="T47" s="4" t="inlineStr"/>
       <c r="U47" s="4" t="inlineStr"/>
@@ -3962,67 +4105,70 @@
       <c r="Z47" s="4" t="inlineStr"/>
       <c r="AA47" s="4" t="inlineStr"/>
       <c r="AB47" s="4" t="inlineStr"/>
-      <c r="AC47" s="5" t="n"/>
+      <c r="AC47" s="4" t="inlineStr"/>
+      <c r="AD47" s="5" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="4" t="inlineStr">
-        <is>
-          <t>NC 2024</t>
-        </is>
-      </c>
-      <c r="B48" s="4" t="inlineStr"/>
-      <c r="C48" s="4" t="inlineStr">
-        <is>
-          <t>BARMM</t>
-        </is>
-      </c>
+      <c r="A48" s="4" t="n">
+        <v>43104</v>
+      </c>
+      <c r="B48" s="4" t="inlineStr">
+        <is>
+          <t>NC 2024</t>
+        </is>
+      </c>
+      <c r="C48" s="4" t="inlineStr"/>
       <c r="D48" s="4" t="inlineStr">
         <is>
+          <t>BARMM</t>
+        </is>
+      </c>
+      <c r="E48" s="4" t="inlineStr">
+        <is>
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="E48" s="4" t="inlineStr"/>
-      <c r="F48" s="4" t="inlineStr">
+      <c r="F48" s="4" t="inlineStr"/>
+      <c r="G48" s="4" t="inlineStr">
         <is>
           <t>Tabawan Stand Alone Senior High School</t>
         </is>
       </c>
-      <c r="G48" s="4" t="inlineStr">
+      <c r="H48" s="4" t="inlineStr">
         <is>
           <t>SOUTH UBIAN</t>
         </is>
       </c>
-      <c r="H48" s="4" t="inlineStr"/>
-      <c r="I48" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="I48" s="4" t="inlineStr"/>
       <c r="J48" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K48" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="K48" s="4" t="inlineStr">
+      <c r="L48" s="4" t="inlineStr">
         <is>
           <t>1STY2CL</t>
         </is>
       </c>
-      <c r="L48" s="4" t="inlineStr">
+      <c r="M48" s="4" t="inlineStr">
         <is>
           <t>GAA 17B</t>
         </is>
       </c>
-      <c r="M48" s="4" t="n">
+      <c r="N48" s="4" t="n">
         <v>5000000</v>
       </c>
-      <c r="N48" s="4" t="inlineStr"/>
       <c r="O48" s="4" t="inlineStr"/>
-      <c r="P48" s="4" t="inlineStr">
+      <c r="P48" s="4" t="inlineStr"/>
+      <c r="Q48" s="4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
         </is>
       </c>
-      <c r="Q48" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R48" s="4" t="inlineStr"/>
+      <c r="R48" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="S48" s="4" t="inlineStr"/>
       <c r="T48" s="4" t="inlineStr"/>
       <c r="U48" s="4" t="inlineStr"/>
@@ -4033,11 +4179,12 @@
       <c r="Z48" s="4" t="inlineStr"/>
       <c r="AA48" s="4" t="inlineStr"/>
       <c r="AB48" s="4" t="inlineStr"/>
-      <c r="AC48" s="5" t="n"/>
+      <c r="AC48" s="4" t="inlineStr"/>
+      <c r="AD48" s="5" t="n"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="AC2:AC48" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AD2:AD48" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>=DropdownOptions!$A$1:$A$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>